<commit_message>
Analyses on IRON LOOP1 updated
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/IRON_LOOP1_UPDATED/AERODYNAMIC_AND_STABILITY_CRUISE/Aerodynamic_and_Stability_CRUISE.xlsx
+++ b/JPADSandBox_v2/out/IRON_LOOP1_UPDATED/AERODYNAMIC_AND_STABILITY_CRUISE/Aerodynamic_and_Stability_CRUISE.xlsx
@@ -7307,97 +7307,97 @@
         <v>5</v>
       </c>
       <c r="C82" t="n">
-        <v>0.020225326890872985</v>
+        <v>0.005825929922538228</v>
       </c>
       <c r="D82" t="n">
-        <v>0.019940155645697524</v>
+        <v>0.005459440976818556</v>
       </c>
       <c r="E82" t="n">
-        <v>0.01967374529344249</v>
+        <v>0.005260466852366906</v>
       </c>
       <c r="F82" t="n">
-        <v>0.019438798768858522</v>
+        <v>0.005241710483933928</v>
       </c>
       <c r="G82" t="n">
-        <v>0.01923186273107272</v>
+        <v>0.005399718530646712</v>
       </c>
       <c r="H82" t="n">
-        <v>0.019050630293971742</v>
+        <v>0.0057321841063919165</v>
       </c>
       <c r="I82" t="n">
-        <v>0.01890307190559326</v>
+        <v>0.006247077659207221</v>
       </c>
       <c r="J82" t="n">
-        <v>0.018779255209096547</v>
+        <v>0.006934466832251891</v>
       </c>
       <c r="K82" t="n">
-        <v>0.018696943072163002</v>
+        <v>0.007812114493207332</v>
       </c>
       <c r="L82" t="n">
-        <v>0.018637744348231185</v>
+        <v>0.008861629495512096</v>
       </c>
       <c r="M82" t="n">
-        <v>0.01861457378584165</v>
+        <v>0.01009592658770675</v>
       </c>
       <c r="N82" t="n">
-        <v>0.018614152988565332</v>
+        <v>0.01150172737336221</v>
       </c>
       <c r="O82" t="n">
-        <v>0.018646182676975466</v>
+        <v>0.013088732573051725</v>
       </c>
       <c r="P82" t="n">
-        <v>0.018702973556179142</v>
+        <v>0.014849252891882384</v>
       </c>
       <c r="Q82" t="n">
-        <v>0.018790562048425743</v>
+        <v>0.016789324752103568</v>
       </c>
       <c r="R82" t="n">
         <v>0.018903087089933823</v>
       </c>
       <c r="S82" t="n">
-        <v>0.01904495491959511</v>
+        <v>0.02119494614426489</v>
       </c>
       <c r="T82" t="n">
-        <v>0.019213860728054366</v>
+        <v>0.023662597105741524</v>
       </c>
       <c r="U82" t="n">
-        <v>0.01941413165446968</v>
+        <v>0.026310367113521815</v>
       </c>
       <c r="V82" t="n">
-        <v>0.01964660041923903</v>
+        <v>0.029139088888003734</v>
       </c>
       <c r="W82" t="n">
-        <v>0.0199088207957795</v>
+        <v>0.032146316202604386</v>
       </c>
       <c r="X82" t="n">
-        <v>0.02020450086268403</v>
+        <v>0.03533575713591669</v>
       </c>
       <c r="Y82" t="n">
-        <v>0.020525107183644777</v>
+        <v>0.03869887825163282</v>
       </c>
       <c r="Z82" t="n">
-        <v>0.020877793295228153</v>
+        <v>0.042242833086319174</v>
       </c>
       <c r="AA82" t="n">
-        <v>0.021254542966279186</v>
+        <v>0.04595960540882078</v>
       </c>
       <c r="AB82" t="n">
-        <v>0.02166425844975125</v>
+        <v>0.04985809747209102</v>
       </c>
       <c r="AC82" t="n">
-        <v>0.022096085599820563</v>
+        <v>0.05392745513030612</v>
       </c>
       <c r="AD82" t="n">
-        <v>0.02256159698647075</v>
+        <v>0.058179250953449675</v>
       </c>
       <c r="AE82" t="n">
-        <v>0.02304938726777251</v>
+        <v>0.06260207959959242</v>
       </c>
       <c r="AF82" t="n">
-        <v>0.02357203979311382</v>
+        <v>0.06720852441812229</v>
       </c>
       <c r="AG82" t="n">
-        <v>0.024119322567493412</v>
+        <v>0.0719830432425292</v>
       </c>
     </row>
     <row r="83">
@@ -11519,7 +11519,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.15853969659117387</v>
+        <v>-0.026240589416081</v>
       </c>
     </row>
     <row r="17">
@@ -17987,97 +17987,97 @@
         <v>5</v>
       </c>
       <c r="C82" t="n">
-        <v>0.005237599496685359</v>
+        <v>0.012221260456910372</v>
       </c>
       <c r="D82" t="n">
-        <v>0.005228006594179508</v>
+        <v>0.011234919718700737</v>
       </c>
       <c r="E82" t="n">
-        <v>0.0052212520952869485</v>
+        <v>0.010453771638654644</v>
       </c>
       <c r="F82" t="n">
-        <v>0.00521536647605533</v>
+        <v>0.009728572134835972</v>
       </c>
       <c r="G82" t="n">
-        <v>0.005209554809839136</v>
+        <v>0.009058008087178574</v>
       </c>
       <c r="H82" t="n">
-        <v>0.005203844508950679</v>
+        <v>0.008441599847089618</v>
       </c>
       <c r="I82" t="n">
-        <v>0.005198366470162428</v>
+        <v>0.007878982300288238</v>
       </c>
       <c r="J82" t="n">
-        <v>0.005194339258354523</v>
+        <v>0.007370888963237522</v>
       </c>
       <c r="K82" t="n">
-        <v>0.005190901449110522</v>
+        <v>0.006915984235291453</v>
       </c>
       <c r="L82" t="n">
-        <v>0.005187562229802654</v>
+        <v>0.006513313908708429</v>
       </c>
       <c r="M82" t="n">
-        <v>0.005184258588374657</v>
+        <v>0.006162362255549783</v>
       </c>
       <c r="N82" t="n">
-        <v>0.005181100015988398</v>
+        <v>0.0058627966293881605</v>
       </c>
       <c r="O82" t="n">
-        <v>0.005179363426853755</v>
+        <v>0.005615462295731007</v>
       </c>
       <c r="P82" t="n">
-        <v>0.0051782280998063195</v>
+        <v>0.0054191172593180586</v>
       </c>
       <c r="Q82" t="n">
-        <v>0.005177095811096593</v>
+        <v>0.005272752293869003</v>
       </c>
       <c r="R82" t="n">
         <v>0.005175966700397133</v>
       </c>
       <c r="S82" t="n">
-        <v>0.0051748390022563024</v>
+        <v>0.005128367929322663</v>
       </c>
       <c r="T82" t="n">
-        <v>0.005174946595406433</v>
+        <v>0.005130809018969658</v>
       </c>
       <c r="U82" t="n">
-        <v>0.005176068830962414</v>
+        <v>0.005182698311650066</v>
       </c>
       <c r="V82" t="n">
-        <v>0.005177186496083082</v>
+        <v>0.005282655304066259</v>
       </c>
       <c r="W82" t="n">
-        <v>0.005178301633050641</v>
+        <v>0.00543033035213811</v>
       </c>
       <c r="X82" t="n">
-        <v>0.005179414088651624</v>
+        <v>0.005625381105280913</v>
       </c>
       <c r="Y82" t="n">
-        <v>0.005181158468572772</v>
+        <v>0.005868109344982558</v>
       </c>
       <c r="Z82" t="n">
-        <v>0.005184223701535731</v>
+        <v>0.006158880432531272</v>
       </c>
       <c r="AA82" t="n">
-        <v>0.005187409953132664</v>
+        <v>0.0064961801059762615</v>
       </c>
       <c r="AB82" t="n">
-        <v>0.005190610292036049</v>
+        <v>0.006879596029107527</v>
       </c>
       <c r="AC82" t="n">
-        <v>0.005193898773527901</v>
+        <v>0.007309420469940458</v>
       </c>
       <c r="AD82" t="n">
-        <v>0.005197569028853467</v>
+        <v>0.007793389146413214</v>
       </c>
       <c r="AE82" t="n">
-        <v>0.0052030128754643485</v>
+        <v>0.00835522608247285</v>
       </c>
       <c r="AF82" t="n">
-        <v>0.0052087800602567</v>
+        <v>0.008972422847771128</v>
       </c>
       <c r="AG82" t="n">
-        <v>0.005215220465368995</v>
+        <v>0.009711166106525757</v>
       </c>
     </row>
     <row r="83">
@@ -22438,97 +22438,97 @@
         <v>5</v>
       </c>
       <c r="C167" t="n">
-        <v>0.00563759949668536</v>
+        <v>0.012621260456910371</v>
       </c>
       <c r="D167" t="n">
-        <v>0.005628006594179508</v>
+        <v>0.011634919718700737</v>
       </c>
       <c r="E167" t="n">
-        <v>0.005621252095286949</v>
+        <v>0.010853771638654643</v>
       </c>
       <c r="F167" t="n">
-        <v>0.00561536647605533</v>
+        <v>0.010128572134835971</v>
       </c>
       <c r="G167" t="n">
-        <v>0.005609554809839136</v>
+        <v>0.009458008087178574</v>
       </c>
       <c r="H167" t="n">
-        <v>0.0056038445089506795</v>
+        <v>0.008841599847089618</v>
       </c>
       <c r="I167" t="n">
-        <v>0.0055983664701624285</v>
+        <v>0.008278982300288238</v>
       </c>
       <c r="J167" t="n">
-        <v>0.005594339258354523</v>
+        <v>0.007770888963237522</v>
       </c>
       <c r="K167" t="n">
-        <v>0.005590901449110522</v>
+        <v>0.007315984235291453</v>
       </c>
       <c r="L167" t="n">
-        <v>0.005587562229802654</v>
+        <v>0.00691331390870843</v>
       </c>
       <c r="M167" t="n">
-        <v>0.005584258588374657</v>
+        <v>0.006562362255549783</v>
       </c>
       <c r="N167" t="n">
-        <v>0.005581100015988398</v>
+        <v>0.006262796629388161</v>
       </c>
       <c r="O167" t="n">
-        <v>0.005579363426853755</v>
+        <v>0.0060154622957310075</v>
       </c>
       <c r="P167" t="n">
-        <v>0.00557822809980632</v>
+        <v>0.005819117259318059</v>
       </c>
       <c r="Q167" t="n">
-        <v>0.005577095811096593</v>
+        <v>0.0056727522938690034</v>
       </c>
       <c r="R167" t="n">
         <v>0.005575966700397133</v>
       </c>
       <c r="S167" t="n">
-        <v>0.005574839002256303</v>
+        <v>0.005528367929322663</v>
       </c>
       <c r="T167" t="n">
-        <v>0.005574946595406433</v>
+        <v>0.0055308090189696586</v>
       </c>
       <c r="U167" t="n">
-        <v>0.005576068830962414</v>
+        <v>0.0055826983116500665</v>
       </c>
       <c r="V167" t="n">
-        <v>0.005577186496083082</v>
+        <v>0.005682655304066259</v>
       </c>
       <c r="W167" t="n">
-        <v>0.005578301633050641</v>
+        <v>0.00583033035213811</v>
       </c>
       <c r="X167" t="n">
-        <v>0.005579414088651624</v>
+        <v>0.006025381105280913</v>
       </c>
       <c r="Y167" t="n">
-        <v>0.005581158468572772</v>
+        <v>0.006268109344982558</v>
       </c>
       <c r="Z167" t="n">
-        <v>0.0055842237015357316</v>
+        <v>0.0065588804325312725</v>
       </c>
       <c r="AA167" t="n">
-        <v>0.005587409953132665</v>
+        <v>0.006896180105976262</v>
       </c>
       <c r="AB167" t="n">
-        <v>0.005590610292036049</v>
+        <v>0.007279596029107527</v>
       </c>
       <c r="AC167" t="n">
-        <v>0.005593898773527901</v>
+        <v>0.007709420469940458</v>
       </c>
       <c r="AD167" t="n">
-        <v>0.0055975690288534675</v>
+        <v>0.008193389146413214</v>
       </c>
       <c r="AE167" t="n">
-        <v>0.005603012875464349</v>
+        <v>0.00875522608247285</v>
       </c>
       <c r="AF167" t="n">
-        <v>0.0056087800602567005</v>
+        <v>0.009372422847771128</v>
       </c>
       <c r="AG167" t="n">
-        <v>0.005615220465368995</v>
+        <v>0.010111166106525757</v>
       </c>
     </row>
     <row r="168">
@@ -23049,7 +23049,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.07256528790779941</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17">
@@ -29430,64 +29430,64 @@
         <v>0.011048396501457728</v>
       </c>
       <c r="D82" t="n">
-        <v>0.011078103619112843</v>
+        <v>0.011746086233236887</v>
       </c>
       <c r="E82" t="n">
-        <v>0.011215749791911556</v>
+        <v>0.013887680248407735</v>
       </c>
       <c r="F82" t="n">
-        <v>0.011443071777984438</v>
+        <v>0.017454915305100835</v>
       </c>
       <c r="G82" t="n">
-        <v>0.011743974488787612</v>
+        <v>0.022431696314772324</v>
       </c>
       <c r="H82" t="n">
-        <v>0.012158139101537771</v>
+        <v>0.028857704454638887</v>
       </c>
       <c r="I82" t="n">
-        <v>0.01262689595266599</v>
+        <v>0.03667427006113158</v>
       </c>
       <c r="J82" t="n">
-        <v>0.013210396726998256</v>
+        <v>0.04594154481907642</v>
       </c>
       <c r="K82" t="n">
-        <v>0.013856548304048345</v>
+        <v>0.056606303382907806</v>
       </c>
       <c r="L82" t="n">
-        <v>0.014603765031795777</v>
+        <v>0.06868923740322262</v>
       </c>
       <c r="M82" t="n">
-        <v>0.015438157079743383</v>
+        <v>0.08213478380239407</v>
       </c>
       <c r="N82" t="n">
-        <v>0.016362791757423244</v>
+        <v>0.09688237351848422</v>
       </c>
       <c r="O82" t="n">
-        <v>0.017386969328977868</v>
+        <v>0.1128525926106235</v>
       </c>
       <c r="P82" t="n">
-        <v>0.01848518483032132</v>
+        <v>0.12990315365651942</v>
       </c>
       <c r="Q82" t="n">
-        <v>0.019678125296596252</v>
+        <v>0.14790723456079363</v>
       </c>
       <c r="R82" t="n">
-        <v>0.020950238751181426</v>
+        <v>0.16666882549662923</v>
       </c>
       <c r="S82" t="n">
-        <v>0.022305524340031156</v>
+        <v>0.1859768506497102</v>
       </c>
       <c r="T82" t="n">
-        <v>0.023761168115793676</v>
+        <v>0.20559781946807126</v>
       </c>
       <c r="U82" t="n">
-        <v>0.02529476237963178</v>
+        <v>0.22522288843892455</v>
       </c>
       <c r="V82" t="n">
-        <v>0.026934752748379316</v>
+        <v>0.2445591335872094</v>
       </c>
       <c r="W82" t="n">
-        <v>0.028648367550039248</v>
+        <v>0.2632194572399567</v>
       </c>
     </row>
     <row r="83">
@@ -33701,64 +33701,64 @@
         <v>0.011448396501457727</v>
       </c>
       <c r="D167" t="n">
-        <v>0.011478103619112843</v>
+        <v>0.012146086233236887</v>
       </c>
       <c r="E167" t="n">
-        <v>0.011615749791911555</v>
+        <v>0.014287680248407734</v>
       </c>
       <c r="F167" t="n">
-        <v>0.011843071777984437</v>
+        <v>0.017854915305100836</v>
       </c>
       <c r="G167" t="n">
-        <v>0.012143974488787611</v>
+        <v>0.022831696314772325</v>
       </c>
       <c r="H167" t="n">
-        <v>0.01255813910153777</v>
+        <v>0.029257704454638888</v>
       </c>
       <c r="I167" t="n">
-        <v>0.01302689595266599</v>
+        <v>0.03707427006113158</v>
       </c>
       <c r="J167" t="n">
-        <v>0.013610396726998255</v>
+        <v>0.046341544819076416</v>
       </c>
       <c r="K167" t="n">
-        <v>0.014256548304048345</v>
+        <v>0.057006303382907804</v>
       </c>
       <c r="L167" t="n">
-        <v>0.015003765031795777</v>
+        <v>0.06908923740322262</v>
       </c>
       <c r="M167" t="n">
-        <v>0.015838157079743384</v>
+        <v>0.08253478380239407</v>
       </c>
       <c r="N167" t="n">
-        <v>0.016762791757423245</v>
+        <v>0.09728237351848422</v>
       </c>
       <c r="O167" t="n">
-        <v>0.01778696932897787</v>
+        <v>0.1132525926106235</v>
       </c>
       <c r="P167" t="n">
-        <v>0.01888518483032132</v>
+        <v>0.13030315365651943</v>
       </c>
       <c r="Q167" t="n">
-        <v>0.020078125296596253</v>
+        <v>0.14830723456079364</v>
       </c>
       <c r="R167" t="n">
-        <v>0.021350238751181427</v>
+        <v>0.16706882549662924</v>
       </c>
       <c r="S167" t="n">
-        <v>0.022705524340031157</v>
+        <v>0.1863768506497102</v>
       </c>
       <c r="T167" t="n">
-        <v>0.024161168115793677</v>
+        <v>0.20599781946807127</v>
       </c>
       <c r="U167" t="n">
-        <v>0.02569476237963178</v>
+        <v>0.22562288843892456</v>
       </c>
       <c r="V167" t="n">
-        <v>0.027334752748379317</v>
+        <v>0.24495913358720942</v>
       </c>
       <c r="W167" t="n">
-        <v>0.02904836755003925</v>
+        <v>0.2636194572399567</v>
       </c>
     </row>
     <row r="168">
@@ -36465,97 +36465,97 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00563759949668536</v>
+        <v>0.012621260456910371</v>
       </c>
       <c r="D8" t="n">
-        <v>0.005628006594179508</v>
+        <v>0.011634919718700737</v>
       </c>
       <c r="E8" t="n">
-        <v>0.005621252095286949</v>
+        <v>0.010853771638654643</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00561536647605533</v>
+        <v>0.010128572134835971</v>
       </c>
       <c r="G8" t="n">
-        <v>0.005609554809839136</v>
+        <v>0.009458008087178574</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0056038445089506795</v>
+        <v>0.008841599847089618</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0055983664701624285</v>
+        <v>0.008278982300288238</v>
       </c>
       <c r="J8" t="n">
-        <v>0.005594339258354523</v>
+        <v>0.007770888963237522</v>
       </c>
       <c r="K8" t="n">
-        <v>0.005590901449110522</v>
+        <v>0.007315984235291453</v>
       </c>
       <c r="L8" t="n">
-        <v>0.005587562229802654</v>
+        <v>0.00691331390870843</v>
       </c>
       <c r="M8" t="n">
-        <v>0.005584258588374657</v>
+        <v>0.006562362255549783</v>
       </c>
       <c r="N8" t="n">
-        <v>0.005581100015988398</v>
+        <v>0.006262796629388161</v>
       </c>
       <c r="O8" t="n">
-        <v>0.005579363426853755</v>
+        <v>0.0060154622957310075</v>
       </c>
       <c r="P8" t="n">
-        <v>0.00557822809980632</v>
+        <v>0.005819117259318059</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.005577095811096593</v>
+        <v>0.0056727522938690034</v>
       </c>
       <c r="R8" t="n">
         <v>0.005575966700397133</v>
       </c>
       <c r="S8" t="n">
-        <v>0.005574839002256303</v>
+        <v>0.005528367929322663</v>
       </c>
       <c r="T8" t="n">
-        <v>0.005574946595406433</v>
+        <v>0.0055308090189696586</v>
       </c>
       <c r="U8" t="n">
-        <v>0.005576068830962414</v>
+        <v>0.0055826983116500665</v>
       </c>
       <c r="V8" t="n">
-        <v>0.005577186496083082</v>
+        <v>0.005682655304066259</v>
       </c>
       <c r="W8" t="n">
-        <v>0.005578301633050641</v>
+        <v>0.00583033035213811</v>
       </c>
       <c r="X8" t="n">
-        <v>0.005579414088651624</v>
+        <v>0.006025381105280913</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.005581158468572772</v>
+        <v>0.006268109344982558</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.0055842237015357316</v>
+        <v>0.0065588804325312725</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.005587409953132665</v>
+        <v>0.006896180105976262</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.005590610292036049</v>
+        <v>0.007279596029107527</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.005593898773527901</v>
+        <v>0.007709420469940458</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.0055975690288534675</v>
+        <v>0.008193389146413214</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.005603012875464349</v>
+        <v>0.00875522608247285</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.0056087800602567005</v>
+        <v>0.009372422847771128</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.005615220465368995</v>
+        <v>0.010111166106525757</v>
       </c>
     </row>
     <row r="9">
@@ -36566,97 +36566,97 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0324691664013625</v>
+        <v>0.020275677151646354</v>
       </c>
       <c r="D9" t="n">
-        <v>0.032058384497777544</v>
+        <v>0.0194750551833597</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03167541944405283</v>
+        <v>0.01891492101539149</v>
       </c>
       <c r="F9" t="n">
-        <v>0.031331890664223296</v>
+        <v>0.018560374905674124</v>
       </c>
       <c r="G9" t="n">
-        <v>0.031025659901472057</v>
+        <v>0.01840911491721313</v>
       </c>
       <c r="H9" t="n">
-        <v>0.030755894650177522</v>
+        <v>0.018460148380603048</v>
       </c>
       <c r="I9" t="n">
-        <v>0.030531985008891357</v>
+        <v>0.018722708720894755</v>
       </c>
       <c r="J9" t="n">
-        <v>0.030345686400765792</v>
+        <v>0.019188398150474212</v>
       </c>
       <c r="K9" t="n">
-        <v>0.030215728031377426</v>
+        <v>0.01987579609831649</v>
       </c>
       <c r="L9" t="n">
-        <v>0.03012474774487963</v>
+        <v>0.02076739403737164</v>
       </c>
       <c r="M9" t="n">
-        <v>0.030086779118304093</v>
+        <v>0.02187708254668432</v>
       </c>
       <c r="N9" t="n">
-        <v>0.030089680037969174</v>
+        <v>0.023192579855919132</v>
       </c>
       <c r="O9" t="n">
-        <v>0.03014462666109648</v>
+        <v>0.024724925778736636</v>
       </c>
       <c r="P9" t="n">
-        <v>0.030244719621629508</v>
+        <v>0.026467087882514673</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0303968385481501</v>
+        <v>0.028425815973717402</v>
       </c>
       <c r="R9" t="n">
         <v>0.0305961428293257</v>
       </c>
       <c r="S9" t="n">
-        <v>0.03084805139834778</v>
+        <v>0.032983363946738654</v>
       </c>
       <c r="T9" t="n">
-        <v>0.031151659281419396</v>
+        <v>0.03558645405725939</v>
       </c>
       <c r="U9" t="n">
-        <v>0.03151223429547261</v>
+        <v>0.03841056378839933</v>
       </c>
       <c r="V9" t="n">
-        <v>0.03193130079449412</v>
+        <v>0.041457103374428976</v>
       </c>
       <c r="W9" t="n">
-        <v>0.03240743239655989</v>
+        <v>0.044724535347324124</v>
       </c>
       <c r="X9" t="n">
-        <v>0.0329453639526008</v>
+        <v>0.04821748646917414</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.033537798503293026</v>
+        <v>0.05192855465248916</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.03419315363955385</v>
+        <v>0.05586605528392668</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.0349040918821931</v>
+        <v>0.06002255156702613</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.035680551317623106</v>
+        <v>0.06440788512088975</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.03651279120402111</v>
+        <v>0.06901238412988628</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.03741369489458577</v>
+        <v>0.07385128265647303</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.038373767544735864</v>
+        <v>0.07892213986212133</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.03940592130880601</v>
+        <v>0.08423121631885269</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.0405022348085368</v>
+        <v>0.08978607614074692</v>
       </c>
     </row>
     <row r="10">
@@ -36778,97 +36778,97 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.3224566230346805</v>
+        <v>-0.3170385632082173</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.3350240026576221</v>
+        <v>-0.3298040683151025</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.3436848479414104</v>
+        <v>-0.3386540755713343</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.35214688117280224</v>
+        <v>-0.34732642821392035</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.36040596577768325</v>
+        <v>-0.355818839334464</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.3684583030625285</v>
+        <v>-0.3641293327131241</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.3763032020618749</v>
+        <v>-0.37225901280255425</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.38393481651217465</v>
+        <v>-0.38020380184122526</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.39135576587905346</v>
+        <v>-0.38796806102259496</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.3985582421566488</v>
+        <v>-0.39554569743817786</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.40512115461335346</v>
+        <v>-0.402517308969809</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.4119072331097898</v>
+        <v>-0.4097472877549697</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.41847053186665323</v>
+        <v>-0.4167913241017333</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.4248068166397743</v>
+        <v>-0.4236467938143769</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.43091595875473176</v>
+        <v>-0.4303151523776042</v>
       </c>
       <c r="R13" t="n">
         <v>-0.4367943573389891</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.4424415568351248</v>
+        <v>-0.4430854859726366</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.4478551456011051</v>
+        <v>-0.4491876340297849</v>
       </c>
       <c r="U13" t="n">
-        <v>-0.45303490209785163</v>
+        <v>-0.4551020620763901</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.4579796930179511</v>
+        <v>-0.4608290937713428</v>
       </c>
       <c r="W13" t="n">
-        <v>-0.46268743663467654</v>
+        <v>-0.46636807936430164</v>
       </c>
       <c r="X13" t="n">
-        <v>-0.4671580043386858</v>
+        <v>-0.4717202973803325</v>
       </c>
       <c r="Y13" t="n">
-        <v>-0.47138766348187555</v>
+        <v>-0.4768833976106742</v>
       </c>
       <c r="Z13" t="n">
-        <v>-0.4753775414405221</v>
+        <v>-0.48185986532160535</v>
       </c>
       <c r="AA13" t="n">
-        <v>-0.47912428898100573</v>
+        <v>-0.4866476847645728</v>
       </c>
       <c r="AB13" t="n">
-        <v>-0.48262977106264493</v>
+        <v>-0.49125003012197166</v>
       </c>
       <c r="AC13" t="n">
-        <v>-0.48591356679531206</v>
+        <v>-0.4956877754485778</v>
       </c>
       <c r="AD13" t="n">
-        <v>-0.489293117739829</v>
+        <v>-0.5002798470087133</v>
       </c>
       <c r="AE13" t="n">
-        <v>-0.4935311513749189</v>
+        <v>-0.5057912134351216</v>
       </c>
       <c r="AF13" t="n">
-        <v>-0.4976378266240218</v>
+        <v>-0.511233096256428</v>
       </c>
       <c r="AG13" t="n">
-        <v>-0.5032874227359647</v>
+        <v>-0.518282996776015</v>
       </c>
     </row>
     <row r="14">
@@ -36889,97 +36889,97 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.3430633702596013</v>
+        <v>-0.33739013798932904</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.3398401199514883</v>
+        <v>-0.3343831514734504</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.33300890448905196</v>
+        <v>-0.3277644390509506</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.32597552309302924</v>
+        <v>-0.3209679044527235</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.31873772815736856</v>
+        <v>-0.3139921038934434</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.3112936264149734</v>
+        <v>-0.306835921458652</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.3036445108969419</v>
+        <v>-0.29950140133379116</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.2957863167765584</v>
+        <v>-0.2919852039210199</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.28772361461170304</v>
+        <v>-0.28429259935694134</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.27945030326335013</v>
+        <v>-0.27641816070829955</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.27054713304067624</v>
+        <v>-0.2679432873971317</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.26187860120585754</v>
+        <v>-0.259733100986539</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.25300052288987823</v>
+        <v>-0.25134401637728937</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.24391043432095572</v>
+        <v>-0.24277414532057184</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.23460990943251578</v>
+        <v>-0.23402561330946</v>
       </c>
       <c r="R16" t="n">
         <v>-0.22509710488970386</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.21537322416364135</v>
+        <v>-0.21599032801848916</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.20543755177200362</v>
+        <v>-0.20670504858951622</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.1952914562860838</v>
+        <v>-0.19724309372435195</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.18493541061562538</v>
+        <v>-0.1876053723411388</v>
       </c>
       <c r="W16" t="n">
-        <v>-0.1743689778029961</v>
+        <v>-0.17779186123204466</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.16359353353151126</v>
+        <v>-0.16780432785408636</v>
       </c>
       <c r="Y16" t="n">
-        <v>-0.1526071011932012</v>
+        <v>-0.15764116567845526</v>
       </c>
       <c r="Z16" t="n">
-        <v>-0.1414121869459322</v>
+        <v>-0.14730522952809486</v>
       </c>
       <c r="AA16" t="n">
-        <v>-0.13000720025705081</v>
+        <v>-0.13679525640055912</v>
       </c>
       <c r="AB16" t="n">
-        <v>-0.11839527300566416</v>
+        <v>-0.12611468484812127</v>
       </c>
       <c r="AC16" t="n">
-        <v>-0.1065959104577282</v>
+        <v>-0.11528331063481809</v>
       </c>
       <c r="AD16" t="n">
-        <v>-0.09490231687201903</v>
+        <v>-0.10459473964494634</v>
       </c>
       <c r="AE16" t="n">
-        <v>-0.08401737639475734</v>
+        <v>-0.09475282086946804</v>
       </c>
       <c r="AF16" t="n">
-        <v>-0.07303233460735464</v>
+        <v>-0.08484907472668929</v>
       </c>
       <c r="AG16" t="n">
-        <v>-0.06476270339701595</v>
+        <v>-0.07770058192943818</v>
       </c>
     </row>
     <row r="17">
@@ -37207,97 +37207,97 @@
         <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>0.005237599496685359</v>
+        <v>0.012221260456910372</v>
       </c>
       <c r="D22" t="n">
-        <v>0.005228006594179508</v>
+        <v>0.011234919718700737</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0052212520952869485</v>
+        <v>0.010453771638654644</v>
       </c>
       <c r="F22" t="n">
-        <v>0.00521536647605533</v>
+        <v>0.009728572134835972</v>
       </c>
       <c r="G22" t="n">
-        <v>0.005209554809839136</v>
+        <v>0.009058008087178574</v>
       </c>
       <c r="H22" t="n">
-        <v>0.005203844508950679</v>
+        <v>0.008441599847089618</v>
       </c>
       <c r="I22" t="n">
-        <v>0.005198366470162428</v>
+        <v>0.007878982300288238</v>
       </c>
       <c r="J22" t="n">
-        <v>0.005194339258354523</v>
+        <v>0.007370888963237522</v>
       </c>
       <c r="K22" t="n">
-        <v>0.005190901449110522</v>
+        <v>0.006915984235291453</v>
       </c>
       <c r="L22" t="n">
-        <v>0.005187562229802654</v>
+        <v>0.006513313908708429</v>
       </c>
       <c r="M22" t="n">
-        <v>0.005184258588374657</v>
+        <v>0.006162362255549783</v>
       </c>
       <c r="N22" t="n">
-        <v>0.005181100015988398</v>
+        <v>0.0058627966293881605</v>
       </c>
       <c r="O22" t="n">
-        <v>0.005179363426853755</v>
+        <v>0.005615462295731007</v>
       </c>
       <c r="P22" t="n">
-        <v>0.0051782280998063195</v>
+        <v>0.0054191172593180586</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.005177095811096593</v>
+        <v>0.005272752293869003</v>
       </c>
       <c r="R22" t="n">
         <v>0.005175966700397133</v>
       </c>
       <c r="S22" t="n">
-        <v>0.0051748390022563024</v>
+        <v>0.005128367929322663</v>
       </c>
       <c r="T22" t="n">
-        <v>0.005174946595406433</v>
+        <v>0.005130809018969658</v>
       </c>
       <c r="U22" t="n">
-        <v>0.005176068830962414</v>
+        <v>0.005182698311650066</v>
       </c>
       <c r="V22" t="n">
-        <v>0.005177186496083082</v>
+        <v>0.005282655304066259</v>
       </c>
       <c r="W22" t="n">
-        <v>0.005178301633050641</v>
+        <v>0.00543033035213811</v>
       </c>
       <c r="X22" t="n">
-        <v>0.005179414088651624</v>
+        <v>0.005625381105280913</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.005181158468572772</v>
+        <v>0.005868109344982558</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.005184223701535731</v>
+        <v>0.006158880432531272</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.005187409953132664</v>
+        <v>0.0064961801059762615</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.005190610292036049</v>
+        <v>0.006879596029107527</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.005193898773527901</v>
+        <v>0.007309420469940458</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.005197569028853467</v>
+        <v>0.007793389146413214</v>
       </c>
       <c r="AE22" t="n">
-        <v>0.0052030128754643485</v>
+        <v>0.00835522608247285</v>
       </c>
       <c r="AF22" t="n">
-        <v>0.0052087800602567</v>
+        <v>0.008972422847771128</v>
       </c>
       <c r="AG22" t="n">
-        <v>0.005215220465368995</v>
+        <v>0.009711166106525757</v>
       </c>
     </row>
     <row r="23">
@@ -37308,97 +37308,97 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.03234281961957099</v>
+        <v>0.02014933036985484</v>
       </c>
       <c r="D23" t="n">
-        <v>0.03193203771598604</v>
+        <v>0.019348708401568188</v>
       </c>
       <c r="E23" t="n">
-        <v>0.03154907266226133</v>
+        <v>0.018788574233599982</v>
       </c>
       <c r="F23" t="n">
-        <v>0.031205543882431783</v>
+        <v>0.018434028123882618</v>
       </c>
       <c r="G23" t="n">
-        <v>0.030899313119680544</v>
+        <v>0.01828276813542162</v>
       </c>
       <c r="H23" t="n">
-        <v>0.03062954786838601</v>
+        <v>0.018333801598811535</v>
       </c>
       <c r="I23" t="n">
-        <v>0.030405638227099845</v>
+        <v>0.018596361939103245</v>
       </c>
       <c r="J23" t="n">
-        <v>0.03021933961897428</v>
+        <v>0.019062051368682702</v>
       </c>
       <c r="K23" t="n">
-        <v>0.030089381249585913</v>
+        <v>0.01974944931652498</v>
       </c>
       <c r="L23" t="n">
-        <v>0.029998400963088125</v>
+        <v>0.020641047255580126</v>
       </c>
       <c r="M23" t="n">
-        <v>0.02996043233651258</v>
+        <v>0.02175073576489281</v>
       </c>
       <c r="N23" t="n">
-        <v>0.02996333325617766</v>
+        <v>0.023066233074127623</v>
       </c>
       <c r="O23" t="n">
-        <v>0.030018279879304968</v>
+        <v>0.024598578996945123</v>
       </c>
       <c r="P23" t="n">
-        <v>0.030118372839837995</v>
+        <v>0.02634074110072316</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.030270491766358588</v>
+        <v>0.02829946919192589</v>
       </c>
       <c r="R23" t="n">
         <v>0.03046979604753419</v>
       </c>
       <c r="S23" t="n">
-        <v>0.030721704616556267</v>
+        <v>0.03285701716494714</v>
       </c>
       <c r="T23" t="n">
-        <v>0.031025312499627884</v>
+        <v>0.035460107275467875</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0313858875136811</v>
+        <v>0.038284217006607814</v>
       </c>
       <c r="V23" t="n">
-        <v>0.031804954012702606</v>
+        <v>0.04133075659263747</v>
       </c>
       <c r="W23" t="n">
-        <v>0.032281085614768376</v>
+        <v>0.04459818856553261</v>
       </c>
       <c r="X23" t="n">
-        <v>0.032819017170809296</v>
+        <v>0.048091139687382635</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.03341145172150152</v>
+        <v>0.051802207870697656</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.03406680685776234</v>
+        <v>0.055739708502135166</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.03477774510040159</v>
+        <v>0.05989620478523462</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.035554204535831586</v>
+        <v>0.06428153833909823</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.036386444422229595</v>
+        <v>0.06888603734809476</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.037287348112794265</v>
+        <v>0.07372493587468153</v>
       </c>
       <c r="AE23" t="n">
-        <v>0.03824742076294435</v>
+        <v>0.07879579308032983</v>
       </c>
       <c r="AF23" t="n">
-        <v>0.03927957452701449</v>
+        <v>0.08410486953706119</v>
       </c>
       <c r="AG23" t="n">
-        <v>0.04037588802674529</v>
+        <v>0.0896597293589554</v>
       </c>
     </row>
     <row r="24">
@@ -37520,97 +37520,97 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.03492899498176966</v>
+        <v>-0.029510935155306395</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.04716705719953812</v>
+        <v>-0.04194712285701857</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.05551254639427275</v>
+        <v>-0.050481774024196596</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.06367320022274119</v>
+        <v>-0.05885274726385929</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.07164489679963615</v>
+        <v>-0.06705777035641691</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.07942385143831972</v>
+        <v>-0.07509488108891522</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.08700938649761306</v>
+        <v>-0.08296519723829238</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.09439566835500102</v>
+        <v>-0.0906646536840516</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.10158532843327382</v>
+        <v>-0.09819762357681529</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.1085705699992826</v>
+        <v>-0.10555802528081165</v>
       </c>
       <c r="M27" t="n">
-        <v>-0.11493031290913336</v>
+        <v>-0.11232646726558884</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.12152729692564565</v>
+        <v>-0.11936735157082562</v>
       </c>
       <c r="O27" t="n">
-        <v>-0.12791558548571316</v>
+        <v>-0.1262363777207932</v>
       </c>
       <c r="P27" t="n">
-        <v>-0.13409095287491624</v>
+        <v>-0.1329309300495188</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.14005327826172018</v>
+        <v>-0.13945247188459262</v>
       </c>
       <c r="R27" t="n">
         <v>-0.1457989679292286</v>
       </c>
       <c r="S27" t="n">
-        <v>-0.1513275727880654</v>
+        <v>-0.15197150192557718</v>
       </c>
       <c r="T27" t="n">
-        <v>-0.15663668697633204</v>
+        <v>-0.15796917540501176</v>
       </c>
       <c r="U27" t="n">
-        <v>-0.16172609404689364</v>
+        <v>-0.16379325402543202</v>
       </c>
       <c r="V27" t="n">
-        <v>-0.16659466509584048</v>
+        <v>-0.16944406584923222</v>
       </c>
       <c r="W27" t="n">
-        <v>-0.17124032211129486</v>
+        <v>-0.17492096484091996</v>
       </c>
       <c r="X27" t="n">
-        <v>-0.17566293950992756</v>
+        <v>-0.1802252325515743</v>
       </c>
       <c r="Y27" t="n">
-        <v>-0.1798587869806658</v>
+        <v>-0.18535452110946446</v>
       </c>
       <c r="Z27" t="n">
-        <v>-0.18382899354771898</v>
+        <v>-0.1903113174288023</v>
       </c>
       <c r="AA27" t="n">
-        <v>-0.18757021093622334</v>
+        <v>-0.19509360671979037</v>
       </c>
       <c r="AB27" t="n">
-        <v>-0.191084304375029</v>
+        <v>-0.19970456343435572</v>
       </c>
       <c r="AC27" t="n">
-        <v>-0.194390852554303</v>
+        <v>-0.20416506120756878</v>
       </c>
       <c r="AD27" t="n">
-        <v>-0.19780729592594518</v>
+        <v>-0.20879402519482967</v>
       </c>
       <c r="AE27" t="n">
-        <v>-0.20209636017059365</v>
+        <v>-0.2143564222307965</v>
       </c>
       <c r="AF27" t="n">
-        <v>-0.2062682017245289</v>
+        <v>-0.2198634713569351</v>
       </c>
       <c r="AG27" t="n">
-        <v>-0.21199709666046357</v>
+        <v>-0.22699267070051404</v>
       </c>
     </row>
     <row r="28">
@@ -37631,97 +37631,97 @@
         <v>5</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.07896462596953183</v>
+        <v>-0.07329139369925955</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.0754231900236312</v>
+        <v>-0.06996622154559336</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.06828660780623871</v>
+        <v>-0.0630421423681373</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.06096069342123604</v>
+        <v>-0.0559530747809303</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.053443213520216803</v>
+        <v>-0.04869758925629172</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.045732288467535354</v>
+        <v>-0.041274583511213936</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.03782922429888119</v>
+        <v>-0.033686114735730466</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.029729968564637804</v>
+        <v>-0.025928855709099252</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.02143910357168826</v>
+        <v>-0.018008088316926567</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.012950539301341244</v>
+        <v>-0.009918396746290668</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.0038450365538970493</v>
+        <v>-0.0012411909103525187</v>
       </c>
       <c r="N30" t="n">
-        <v>0.00501289754706633</v>
+        <v>0.007158397766384791</v>
       </c>
       <c r="O30" t="n">
-        <v>0.014067438639365468</v>
+        <v>0.015723945151954345</v>
       </c>
       <c r="P30" t="n">
-        <v>0.023321041894236155</v>
+        <v>0.024457330894620013</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.03277212540877753</v>
+        <v>0.033356421531833304</v>
       </c>
       <c r="R30" t="n">
         <v>0.042422525179829126</v>
       </c>
       <c r="S30" t="n">
-        <v>0.05227103103007225</v>
+        <v>0.05165392717522446</v>
       </c>
       <c r="T30" t="n">
-        <v>0.06231835236777876</v>
+        <v>0.06105085555026619</v>
       </c>
       <c r="U30" t="n">
-        <v>0.0725631151800436</v>
+        <v>0.0706114777417754</v>
       </c>
       <c r="V30" t="n">
-        <v>0.08300484174821651</v>
+        <v>0.08033488002270309</v>
       </c>
       <c r="W30" t="n">
-        <v>0.09364396485396412</v>
+        <v>0.09022108142491557</v>
       </c>
       <c r="X30" t="n">
-        <v>0.10447910527114881</v>
+        <v>0.1002683109485736</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.11551223669823406</v>
+        <v>0.11047817221297998</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.12674085070130592</v>
+        <v>0.12084780811914325</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.13816653617053948</v>
+        <v>0.13137848002703112</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.14978616021799812</v>
+        <v>0.14206674837554104</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.1615802172025949</v>
+        <v>0.1528928170255051</v>
       </c>
       <c r="AD30" t="n">
-        <v>0.17325550312413943</v>
+        <v>0.16356308035121211</v>
       </c>
       <c r="AE30" t="n">
-        <v>0.18410913472870077</v>
+        <v>0.1733736902539901</v>
       </c>
       <c r="AF30" t="n">
-        <v>0.19504986796081755</v>
+        <v>0.18323312784148302</v>
       </c>
       <c r="AG30" t="n">
-        <v>0.2032621930928214</v>
+        <v>0.19032431456039933</v>
       </c>
     </row>
     <row r="31">
@@ -37949,97 +37949,97 @@
         <v>5</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0056175994966853595</v>
+        <v>0.012601260456910372</v>
       </c>
       <c r="D36" t="n">
-        <v>0.005608006594179508</v>
+        <v>0.011614919718700737</v>
       </c>
       <c r="E36" t="n">
-        <v>0.005601252095286949</v>
+        <v>0.010833771638654644</v>
       </c>
       <c r="F36" t="n">
-        <v>0.00559536647605533</v>
+        <v>0.010108572134835972</v>
       </c>
       <c r="G36" t="n">
-        <v>0.005589554809839136</v>
+        <v>0.009438008087178575</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0055838445089506795</v>
+        <v>0.008821599847089618</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0055783664701624285</v>
+        <v>0.008258982300288239</v>
       </c>
       <c r="J36" t="n">
-        <v>0.005574339258354523</v>
+        <v>0.007750888963237522</v>
       </c>
       <c r="K36" t="n">
-        <v>0.005570901449110522</v>
+        <v>0.007295984235291453</v>
       </c>
       <c r="L36" t="n">
-        <v>0.005567562229802654</v>
+        <v>0.0068933139087084296</v>
       </c>
       <c r="M36" t="n">
-        <v>0.005564258588374657</v>
+        <v>0.006542362255549783</v>
       </c>
       <c r="N36" t="n">
-        <v>0.005561100015988398</v>
+        <v>0.006242796629388161</v>
       </c>
       <c r="O36" t="n">
-        <v>0.005559363426853755</v>
+        <v>0.005995462295731007</v>
       </c>
       <c r="P36" t="n">
-        <v>0.00555822809980632</v>
+        <v>0.005799117259318059</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.005557095811096593</v>
+        <v>0.005652752293869003</v>
       </c>
       <c r="R36" t="n">
         <v>0.005555966700397133</v>
       </c>
       <c r="S36" t="n">
-        <v>0.005554839002256303</v>
+        <v>0.005508367929322663</v>
       </c>
       <c r="T36" t="n">
-        <v>0.005554946595406433</v>
+        <v>0.0055108090189696585</v>
       </c>
       <c r="U36" t="n">
-        <v>0.005556068830962414</v>
+        <v>0.0055626983116500665</v>
       </c>
       <c r="V36" t="n">
-        <v>0.005557186496083082</v>
+        <v>0.005662655304066259</v>
       </c>
       <c r="W36" t="n">
-        <v>0.005558301633050641</v>
+        <v>0.00581033035213811</v>
       </c>
       <c r="X36" t="n">
-        <v>0.005559414088651624</v>
+        <v>0.006005381105280913</v>
       </c>
       <c r="Y36" t="n">
-        <v>0.005561158468572772</v>
+        <v>0.006248109344982558</v>
       </c>
       <c r="Z36" t="n">
-        <v>0.0055642237015357315</v>
+        <v>0.0065388804325312725</v>
       </c>
       <c r="AA36" t="n">
-        <v>0.0055674099531326645</v>
+        <v>0.006876180105976262</v>
       </c>
       <c r="AB36" t="n">
-        <v>0.005570610292036049</v>
+        <v>0.007259596029107527</v>
       </c>
       <c r="AC36" t="n">
-        <v>0.005573898773527901</v>
+        <v>0.007689420469940458</v>
       </c>
       <c r="AD36" t="n">
-        <v>0.0055775690288534675</v>
+        <v>0.008173389146413215</v>
       </c>
       <c r="AE36" t="n">
-        <v>0.005583012875464349</v>
+        <v>0.00873522608247285</v>
       </c>
       <c r="AF36" t="n">
-        <v>0.0055887800602567005</v>
+        <v>0.009352422847771128</v>
       </c>
       <c r="AG36" t="n">
-        <v>0.005595220465368995</v>
+        <v>0.010091166106525757</v>
       </c>
     </row>
     <row r="37">
@@ -38050,97 +38050,97 @@
         <v>5</v>
       </c>
       <c r="C37" t="n">
-        <v>0.032462849062272925</v>
+        <v>0.02026935981255678</v>
       </c>
       <c r="D37" t="n">
-        <v>0.03205206715868797</v>
+        <v>0.019468737844270126</v>
       </c>
       <c r="E37" t="n">
-        <v>0.03166910210496326</v>
+        <v>0.018908603676301917</v>
       </c>
       <c r="F37" t="n">
-        <v>0.031325573325133714</v>
+        <v>0.01855405756658455</v>
       </c>
       <c r="G37" t="n">
-        <v>0.031019342562382483</v>
+        <v>0.018402797578123554</v>
       </c>
       <c r="H37" t="n">
-        <v>0.03074957731108794</v>
+        <v>0.01845383104151347</v>
       </c>
       <c r="I37" t="n">
-        <v>0.030525667669801783</v>
+        <v>0.01871639138180518</v>
       </c>
       <c r="J37" t="n">
-        <v>0.030339369061676218</v>
+        <v>0.019182080811384637</v>
       </c>
       <c r="K37" t="n">
-        <v>0.03020941069228785</v>
+        <v>0.019869478759226913</v>
       </c>
       <c r="L37" t="n">
-        <v>0.030118430405790056</v>
+        <v>0.020761076698282064</v>
       </c>
       <c r="M37" t="n">
-        <v>0.03008046177921451</v>
+        <v>0.021870765207594744</v>
       </c>
       <c r="N37" t="n">
-        <v>0.0300833626988796</v>
+        <v>0.023186262516829557</v>
       </c>
       <c r="O37" t="n">
-        <v>0.030138309322006906</v>
+        <v>0.02471860843964706</v>
       </c>
       <c r="P37" t="n">
-        <v>0.030238402282539933</v>
+        <v>0.026460770543425098</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.030390521209060526</v>
+        <v>0.028419498634627827</v>
       </c>
       <c r="R37" t="n">
         <v>0.030589825490236127</v>
       </c>
       <c r="S37" t="n">
-        <v>0.030841734059258205</v>
+        <v>0.03297704660764908</v>
       </c>
       <c r="T37" t="n">
-        <v>0.031145341942329822</v>
+        <v>0.035580136718169814</v>
       </c>
       <c r="U37" t="n">
-        <v>0.03150591695638303</v>
+        <v>0.03840424644930975</v>
       </c>
       <c r="V37" t="n">
-        <v>0.031924983455404544</v>
+        <v>0.0414507860353394</v>
       </c>
       <c r="W37" t="n">
-        <v>0.032401115057470314</v>
+        <v>0.04471821800823455</v>
       </c>
       <c r="X37" t="n">
-        <v>0.03293904661351122</v>
+        <v>0.04821116913008457</v>
       </c>
       <c r="Y37" t="n">
-        <v>0.03353148116420346</v>
+        <v>0.05192223731339958</v>
       </c>
       <c r="Z37" t="n">
-        <v>0.03418683630046428</v>
+        <v>0.055859737944837104</v>
       </c>
       <c r="AA37" t="n">
-        <v>0.03489777454310353</v>
+        <v>0.06001623422793655</v>
       </c>
       <c r="AB37" t="n">
-        <v>0.035674233978533525</v>
+        <v>0.06440156778180017</v>
       </c>
       <c r="AC37" t="n">
-        <v>0.036506473864931534</v>
+        <v>0.0690060667907967</v>
       </c>
       <c r="AD37" t="n">
-        <v>0.03740737755549619</v>
+        <v>0.07384496531738345</v>
       </c>
       <c r="AE37" t="n">
-        <v>0.03836745020564629</v>
+        <v>0.07891582252303175</v>
       </c>
       <c r="AF37" t="n">
-        <v>0.03939960396971643</v>
+        <v>0.08422489897976311</v>
       </c>
       <c r="AG37" t="n">
-        <v>0.04049591746944722</v>
+        <v>0.08977975880165734</v>
       </c>
     </row>
     <row r="38">
@@ -38262,97 +38262,97 @@
         <v>5</v>
       </c>
       <c r="C41" t="n">
-        <v>0.25274876608517793</v>
+        <v>0.258166825911641</v>
       </c>
       <c r="D41" t="n">
-        <v>0.24083373030601107</v>
+        <v>0.24605366464853062</v>
       </c>
       <c r="E41" t="n">
-        <v>0.2327972992234333</v>
+        <v>0.23782807159350963</v>
       </c>
       <c r="F41" t="n">
-        <v>0.2249317201176213</v>
+        <v>0.22975217307650314</v>
       </c>
       <c r="G41" t="n">
-        <v>0.21724110049235584</v>
+        <v>0.22182822693557525</v>
       </c>
       <c r="H41" t="n">
-        <v>0.20972921133498157</v>
+        <v>0.21405818168438612</v>
       </c>
       <c r="I41" t="n">
-        <v>0.2023967172702819</v>
+        <v>0.20644090652960273</v>
       </c>
       <c r="J41" t="n">
-        <v>0.19524943958791116</v>
+        <v>0.19898045425886063</v>
       </c>
       <c r="K41" t="n">
-        <v>0.1882847352163528</v>
+        <v>0.19167244007281137</v>
       </c>
       <c r="L41" t="n">
-        <v>0.1815103899247319</v>
+        <v>0.18452293464320277</v>
       </c>
       <c r="M41" t="n">
-        <v>0.17534747357815547</v>
+        <v>0.1779513192217</v>
       </c>
       <c r="N41" t="n">
-        <v>0.16893323682075512</v>
+        <v>0.1710931821755751</v>
       </c>
       <c r="O41" t="n">
-        <v>0.16271360730879342</v>
+        <v>0.16439281507371337</v>
       </c>
       <c r="P41" t="n">
-        <v>0.15669280253648588</v>
+        <v>0.1578528253618834</v>
       </c>
       <c r="Q41" t="n">
-        <v>0.15087093580220365</v>
+        <v>0.1514717421793312</v>
       </c>
       <c r="R41" t="n">
         <v>0.1452515939770863</v>
       </c>
       <c r="S41" t="n">
-        <v>0.13983521999249438</v>
+        <v>0.13919129085498258</v>
       </c>
       <c r="T41" t="n">
-        <v>0.1346242142403521</v>
+        <v>0.13329172581167226</v>
       </c>
       <c r="U41" t="n">
-        <v>0.12961878838612725</v>
+        <v>0.12755162840758885</v>
       </c>
       <c r="V41" t="n">
-        <v>0.12482006724060382</v>
+        <v>0.12197066648721211</v>
       </c>
       <c r="W41" t="n">
-        <v>0.12023012541127366</v>
+        <v>0.11654948268164857</v>
       </c>
       <c r="X41" t="n">
-        <v>0.11584908576598645</v>
+        <v>0.11128679272433968</v>
       </c>
       <c r="Y41" t="n">
-        <v>0.11168067658937395</v>
+        <v>0.1061849424605753</v>
       </c>
       <c r="Z41" t="n">
-        <v>0.10772376751992291</v>
+        <v>0.10124144363883958</v>
       </c>
       <c r="AA41" t="n">
-        <v>0.10398170618439596</v>
+        <v>0.09645831040082888</v>
       </c>
       <c r="AB41" t="n">
-        <v>0.10045262739507563</v>
+        <v>0.09183236833574884</v>
       </c>
       <c r="AC41" t="n">
-        <v>0.0971169531921598</v>
+        <v>0.087342744538894</v>
       </c>
       <c r="AD41" t="n">
-        <v>0.09365724454330987</v>
+        <v>0.08267051527442543</v>
       </c>
       <c r="AE41" t="n">
-        <v>0.08931077787657637</v>
+        <v>0.07705071581637359</v>
       </c>
       <c r="AF41" t="n">
-        <v>0.08506739955339201</v>
+        <v>0.07147212992098576</v>
       </c>
       <c r="AG41" t="n">
-        <v>0.07925283698764506</v>
+        <v>0.06425726294759466</v>
       </c>
     </row>
     <row r="42">
@@ -38373,97 +38373,97 @@
         <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1852790954335837</v>
+        <v>0.19095232770385587</v>
       </c>
       <c r="D44" t="n">
-        <v>0.18913294092435046</v>
+        <v>0.19458990940238818</v>
       </c>
       <c r="E44" t="n">
-        <v>0.19656910701964928</v>
+        <v>0.2018135724577508</v>
       </c>
       <c r="F44" t="n">
-        <v>0.2041817650143038</v>
+        <v>0.2091893836546096</v>
       </c>
       <c r="G44" t="n">
-        <v>0.21197313428124073</v>
+        <v>0.21671875854516595</v>
       </c>
       <c r="H44" t="n">
-        <v>0.21994508110712493</v>
+        <v>0.2244027860634463</v>
       </c>
       <c r="I44" t="n">
-        <v>0.2280962867344335</v>
+        <v>0.23223939629758422</v>
       </c>
       <c r="J44" t="n">
-        <v>0.23643079151871857</v>
+        <v>0.24023190437425715</v>
       </c>
       <c r="K44" t="n">
-        <v>0.24494400168739022</v>
+        <v>0.24837501694215186</v>
       </c>
       <c r="L44" t="n">
-        <v>0.25364199642234947</v>
+        <v>0.25667413897740005</v>
       </c>
       <c r="M44" t="n">
-        <v>0.2629440047159508</v>
+        <v>0.26554785035949535</v>
       </c>
       <c r="N44" t="n">
-        <v>0.2719855098672131</v>
+        <v>0.2741310100865316</v>
       </c>
       <c r="O44" t="n">
-        <v>0.2812106785669589</v>
+        <v>0.2828671850795477</v>
       </c>
       <c r="P44" t="n">
-        <v>0.2906219576702749</v>
+        <v>0.29175824667065886</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.3002177575893622</v>
+        <v>0.30080205371241797</v>
       </c>
       <c r="R44" t="n">
         <v>0.30999990726778687</v>
       </c>
       <c r="S44" t="n">
-        <v>0.31996719010692537</v>
+        <v>0.3193500862520776</v>
       </c>
       <c r="T44" t="n">
-        <v>0.330120309726027</v>
+        <v>0.3288528129085144</v>
       </c>
       <c r="U44" t="n">
-        <v>0.34045788695572743</v>
+        <v>0.3385062495174593</v>
       </c>
       <c r="V44" t="n">
-        <v>0.3509794395537329</v>
+        <v>0.3483094778282194</v>
       </c>
       <c r="W44" t="n">
-        <v>0.36168539641110165</v>
+        <v>0.35826251298205314</v>
       </c>
       <c r="X44" t="n">
-        <v>0.3725743750443137</v>
+        <v>0.36836358072173836</v>
       </c>
       <c r="Y44" t="n">
-        <v>0.3836483465278334</v>
+        <v>0.3786142820425794</v>
       </c>
       <c r="Z44" t="n">
-        <v>0.3949048004372605</v>
+        <v>0.3890117578550978</v>
       </c>
       <c r="AA44" t="n">
-        <v>0.40634532430589193</v>
+        <v>0.3995572681623835</v>
       </c>
       <c r="AB44" t="n">
-        <v>0.4179667845225886</v>
+        <v>0.4102473726801315</v>
       </c>
       <c r="AC44" t="n">
-        <v>0.42974967535677144</v>
+        <v>0.42106227517968153</v>
       </c>
       <c r="AD44" t="n">
-        <v>0.4414007933524722</v>
+        <v>0.4317083705795448</v>
       </c>
       <c r="AE44" t="n">
-        <v>0.4522172564336706</v>
+        <v>0.44148181195895997</v>
       </c>
       <c r="AF44" t="n">
-        <v>0.4631078223564468</v>
+        <v>0.4512910822371123</v>
       </c>
       <c r="AG44" t="n">
-        <v>0.4712569838382163</v>
+        <v>0.45831910530579417</v>
       </c>
     </row>
     <row r="45">
@@ -38691,97 +38691,97 @@
         <v>5</v>
       </c>
       <c r="C50" t="n">
-        <v>0.006777599496685359</v>
+        <v>0.013761260456910372</v>
       </c>
       <c r="D50" t="n">
-        <v>0.006768006594179508</v>
+        <v>0.012774919718700737</v>
       </c>
       <c r="E50" t="n">
-        <v>0.006761252095286948</v>
+        <v>0.011993771638654643</v>
       </c>
       <c r="F50" t="n">
-        <v>0.006755366476055329</v>
+        <v>0.011268572134835972</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0067495548098391355</v>
+        <v>0.010598008087178574</v>
       </c>
       <c r="H50" t="n">
-        <v>0.006743844508950679</v>
+        <v>0.009981599847089618</v>
       </c>
       <c r="I50" t="n">
-        <v>0.006738366470162428</v>
+        <v>0.009418982300288238</v>
       </c>
       <c r="J50" t="n">
-        <v>0.0067343392583545224</v>
+        <v>0.008910888963237521</v>
       </c>
       <c r="K50" t="n">
-        <v>0.006730901449110521</v>
+        <v>0.008455984235291453</v>
       </c>
       <c r="L50" t="n">
-        <v>0.006727562229802654</v>
+        <v>0.008053313908708429</v>
       </c>
       <c r="M50" t="n">
-        <v>0.006724258588374657</v>
+        <v>0.007702362255549783</v>
       </c>
       <c r="N50" t="n">
-        <v>0.006721100015988398</v>
+        <v>0.00740279662938816</v>
       </c>
       <c r="O50" t="n">
-        <v>0.0067193634268537545</v>
+        <v>0.007155462295731007</v>
       </c>
       <c r="P50" t="n">
-        <v>0.006718228099806319</v>
+        <v>0.006959117259318058</v>
       </c>
       <c r="Q50" t="n">
-        <v>0.006717095811096593</v>
+        <v>0.006812752293869003</v>
       </c>
       <c r="R50" t="n">
         <v>0.006715966700397133</v>
       </c>
       <c r="S50" t="n">
-        <v>0.006714839002256302</v>
+        <v>0.006668367929322663</v>
       </c>
       <c r="T50" t="n">
-        <v>0.006714946595406433</v>
+        <v>0.006670809018969658</v>
       </c>
       <c r="U50" t="n">
-        <v>0.006716068830962414</v>
+        <v>0.006722698311650066</v>
       </c>
       <c r="V50" t="n">
-        <v>0.006717186496083082</v>
+        <v>0.006822655304066259</v>
       </c>
       <c r="W50" t="n">
-        <v>0.006718301633050641</v>
+        <v>0.00697033035213811</v>
       </c>
       <c r="X50" t="n">
-        <v>0.006719414088651623</v>
+        <v>0.007165381105280913</v>
       </c>
       <c r="Y50" t="n">
-        <v>0.006721158468572771</v>
+        <v>0.007408109344982558</v>
       </c>
       <c r="Z50" t="n">
-        <v>0.006724223701535731</v>
+        <v>0.007698880432531272</v>
       </c>
       <c r="AA50" t="n">
-        <v>0.006727409953132664</v>
+        <v>0.008036180105976261</v>
       </c>
       <c r="AB50" t="n">
-        <v>0.006730610292036049</v>
+        <v>0.008419596029107527</v>
       </c>
       <c r="AC50" t="n">
-        <v>0.006733898773527901</v>
+        <v>0.008849420469940458</v>
       </c>
       <c r="AD50" t="n">
-        <v>0.006737569028853467</v>
+        <v>0.009333389146413214</v>
       </c>
       <c r="AE50" t="n">
-        <v>0.006743012875464348</v>
+        <v>0.00989522608247285</v>
       </c>
       <c r="AF50" t="n">
-        <v>0.0067487800602567</v>
+        <v>0.010512422847771128</v>
       </c>
       <c r="AG50" t="n">
-        <v>0.006755220465368994</v>
+        <v>0.011251166106525757</v>
       </c>
     </row>
     <row r="51">
@@ -38792,97 +38792,97 @@
         <v>5</v>
       </c>
       <c r="C51" t="n">
-        <v>0.03282925472946831</v>
+        <v>0.020635765479752162</v>
       </c>
       <c r="D51" t="n">
-        <v>0.03241847282588335</v>
+        <v>0.01983514351146551</v>
       </c>
       <c r="E51" t="n">
-        <v>0.03203550777215864</v>
+        <v>0.019275009343497296</v>
       </c>
       <c r="F51" t="n">
-        <v>0.031691978992329096</v>
+        <v>0.01892046323377993</v>
       </c>
       <c r="G51" t="n">
-        <v>0.03138574822957786</v>
+        <v>0.018769203245318937</v>
       </c>
       <c r="H51" t="n">
-        <v>0.031115982978283323</v>
+        <v>0.018820236708708853</v>
       </c>
       <c r="I51" t="n">
-        <v>0.030892073336997165</v>
+        <v>0.019082797049000563</v>
       </c>
       <c r="J51" t="n">
-        <v>0.0307057747288716</v>
+        <v>0.01954848647858002</v>
       </c>
       <c r="K51" t="n">
-        <v>0.030575816359483234</v>
+        <v>0.020235884426422296</v>
       </c>
       <c r="L51" t="n">
-        <v>0.03048483607298544</v>
+        <v>0.021127482365477446</v>
       </c>
       <c r="M51" t="n">
-        <v>0.030446867446409894</v>
+        <v>0.022237170874790126</v>
       </c>
       <c r="N51" t="n">
-        <v>0.03044976836607498</v>
+        <v>0.023552668184024936</v>
       </c>
       <c r="O51" t="n">
-        <v>0.03050471498920229</v>
+        <v>0.025085014106842444</v>
       </c>
       <c r="P51" t="n">
-        <v>0.03060480794973531</v>
+        <v>0.02682717621062048</v>
       </c>
       <c r="Q51" t="n">
-        <v>0.03075692687625591</v>
+        <v>0.02878590430182321</v>
       </c>
       <c r="R51" t="n">
         <v>0.03095623115743151</v>
       </c>
       <c r="S51" t="n">
-        <v>0.031208139726453588</v>
+        <v>0.03334345227484446</v>
       </c>
       <c r="T51" t="n">
-        <v>0.03151174760952521</v>
+        <v>0.035946542385365196</v>
       </c>
       <c r="U51" t="n">
-        <v>0.03187232262357841</v>
+        <v>0.038770652116505135</v>
       </c>
       <c r="V51" t="n">
-        <v>0.03229138912259993</v>
+        <v>0.041817191702534784</v>
       </c>
       <c r="W51" t="n">
-        <v>0.0327675207246657</v>
+        <v>0.04508462367542993</v>
       </c>
       <c r="X51" t="n">
-        <v>0.0333054522807066</v>
+        <v>0.048577574797279956</v>
       </c>
       <c r="Y51" t="n">
-        <v>0.03389788683139884</v>
+        <v>0.05228864298059496</v>
       </c>
       <c r="Z51" t="n">
-        <v>0.03455324196765966</v>
+        <v>0.056226143612032486</v>
       </c>
       <c r="AA51" t="n">
-        <v>0.03526418021029891</v>
+        <v>0.060382639895131936</v>
       </c>
       <c r="AB51" t="n">
-        <v>0.03604063964572891</v>
+        <v>0.06476797344899556</v>
       </c>
       <c r="AC51" t="n">
-        <v>0.036872879532126916</v>
+        <v>0.06937247245799208</v>
       </c>
       <c r="AD51" t="n">
-        <v>0.03777378322269157</v>
+        <v>0.07421137098457883</v>
       </c>
       <c r="AE51" t="n">
-        <v>0.03873385587284167</v>
+        <v>0.07928222819022714</v>
       </c>
       <c r="AF51" t="n">
-        <v>0.03976600963691181</v>
+        <v>0.08459130464695849</v>
       </c>
       <c r="AG51" t="n">
-        <v>0.0408623231366426</v>
+        <v>0.09014616446885272</v>
       </c>
     </row>
     <row r="52">
@@ -39004,97 +39004,97 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>0.5366426685663884</v>
+        <v>0.5420607283928515</v>
       </c>
       <c r="D55" t="n">
-        <v>0.5250370583334937</v>
+        <v>0.5302569926760131</v>
       </c>
       <c r="E55" t="n">
-        <v>0.5172963905091681</v>
+        <v>0.5223271628792441</v>
       </c>
       <c r="F55" t="n">
-        <v>0.5097128979585037</v>
+        <v>0.5145333509173855</v>
       </c>
       <c r="G55" t="n">
-        <v>0.5022906744367817</v>
+        <v>0.5068778008800009</v>
       </c>
       <c r="H55" t="n">
-        <v>0.4950334778500982</v>
+        <v>0.4993624481995026</v>
       </c>
       <c r="I55" t="n">
-        <v>0.48794196040988064</v>
+        <v>0.49198614966920146</v>
       </c>
       <c r="J55" t="n">
-        <v>0.48102193166092255</v>
+        <v>0.48475294633187205</v>
       </c>
       <c r="K55" t="n">
-        <v>0.4742707374559148</v>
+        <v>0.47765844231237325</v>
       </c>
       <c r="L55" t="n">
-        <v>0.4676961531577982</v>
+        <v>0.4707086978762693</v>
       </c>
       <c r="M55" t="n">
-        <v>0.46171923889561095</v>
+        <v>0.4643230845391555</v>
       </c>
       <c r="N55" t="n">
-        <v>0.4554772362480052</v>
+        <v>0.4576371816028252</v>
       </c>
       <c r="O55" t="n">
-        <v>0.4494160644767963</v>
+        <v>0.45109527224171625</v>
       </c>
       <c r="P55" t="n">
-        <v>0.443539933353193</v>
+        <v>0.4446999561785903</v>
       </c>
       <c r="Q55" t="n">
-        <v>0.4378489491243766</v>
+        <v>0.4384497555015043</v>
       </c>
       <c r="R55" t="n">
         <v>0.43234669228245826</v>
       </c>
       <c r="S55" t="n">
-        <v>0.4270336000522416</v>
+        <v>0.42638967091472996</v>
       </c>
       <c r="T55" t="n">
-        <v>0.4219120677918436</v>
+        <v>0.42057957936316387</v>
       </c>
       <c r="U55" t="n">
-        <v>0.41698230280592086</v>
+        <v>0.41491514282738257</v>
       </c>
       <c r="V55" t="n">
-        <v>0.41224542621765264</v>
+        <v>0.40939602546426107</v>
       </c>
       <c r="W55" t="n">
-        <v>0.4077035096203149</v>
+        <v>0.4040228668906898</v>
       </c>
       <c r="X55" t="n">
-        <v>0.4033566735410751</v>
+        <v>0.3987943804994284</v>
       </c>
       <c r="Y55" t="n">
-        <v>0.39920864459753125</v>
+        <v>0.3937129104687326</v>
       </c>
       <c r="Z55" t="n">
-        <v>0.3952582914348665</v>
+        <v>0.38877596755378324</v>
       </c>
       <c r="AA55" t="n">
-        <v>0.3915089613603178</v>
+        <v>0.3839855655767506</v>
       </c>
       <c r="AB55" t="n">
-        <v>0.3879587895404358</v>
+        <v>0.37933853048110894</v>
       </c>
       <c r="AC55" t="n">
-        <v>0.3845881990434627</v>
+        <v>0.37481399039019697</v>
       </c>
       <c r="AD55" t="n">
-        <v>0.3810797525388312</v>
+        <v>0.37009302326994675</v>
       </c>
       <c r="AE55" t="n">
-        <v>0.37667072883000596</v>
+        <v>0.36441066676980316</v>
       </c>
       <c r="AF55" t="n">
-        <v>0.37235097732736155</v>
+        <v>0.3587557076949552</v>
       </c>
       <c r="AG55" t="n">
-        <v>0.36644622916710734</v>
+        <v>0.351450655127057</v>
       </c>
     </row>
     <row r="56">
@@ -39115,97 +39115,97 @@
         <v>5</v>
       </c>
       <c r="C58" t="n">
-        <v>0.4462590624390388</v>
+        <v>0.45193229470931096</v>
       </c>
       <c r="D58" t="n">
-        <v>0.45041247507581333</v>
+        <v>0.4558694435538511</v>
       </c>
       <c r="E58" t="n">
-        <v>0.458135663302473</v>
+        <v>0.46338012874057455</v>
       </c>
       <c r="F58" t="n">
-        <v>0.46602278442478723</v>
+        <v>0.47103040306509264</v>
       </c>
       <c r="G58" t="n">
-        <v>0.4740760444387371</v>
+        <v>0.4788216687026623</v>
       </c>
       <c r="H58" t="n">
-        <v>0.4822972968668022</v>
+        <v>0.4867550018231237</v>
       </c>
       <c r="I58" t="n">
-        <v>0.49068521080065614</v>
+        <v>0.49482832036380703</v>
       </c>
       <c r="J58" t="n">
-        <v>0.4992438150590224</v>
+        <v>0.5030449279145608</v>
       </c>
       <c r="K58" t="n">
-        <v>0.5079685049470182</v>
+        <v>0.5113995202017798</v>
       </c>
       <c r="L58" t="n">
-        <v>0.516865349339322</v>
+        <v>0.5198974918943725</v>
       </c>
       <c r="M58" t="n">
-        <v>0.5263535675366362</v>
+        <v>0.5289574131801807</v>
       </c>
       <c r="N58" t="n">
-        <v>0.5355686337623717</v>
+        <v>0.5377141339816901</v>
       </c>
       <c r="O58" t="n">
-        <v>0.5449547062482294</v>
+        <v>0.5466112127608181</v>
       </c>
       <c r="P58" t="n">
-        <v>0.5545142240070723</v>
+        <v>0.5556505130074563</v>
       </c>
       <c r="Q58" t="n">
-        <v>0.5642455902261586</v>
+        <v>0.5648298863492144</v>
       </c>
       <c r="R58" t="n">
         <v>0.5741506272417441</v>
       </c>
       <c r="S58" t="n">
-        <v>0.5842281124658497</v>
+        <v>0.5836110086110019</v>
       </c>
       <c r="T58" t="n">
-        <v>0.5944787441466161</v>
+        <v>0.5932112473291034</v>
       </c>
       <c r="U58" t="n">
-        <v>0.6049011383620786</v>
+        <v>0.6029495009238104</v>
       </c>
       <c r="V58" t="n">
-        <v>0.6154948087360832</v>
+        <v>0.6128248470105697</v>
       </c>
       <c r="W58" t="n">
-        <v>0.6262601806447696</v>
+        <v>0.622837297215721</v>
       </c>
       <c r="X58" t="n">
-        <v>0.6371958687088118</v>
+        <v>0.6329850743862366</v>
       </c>
       <c r="Y58" t="n">
-        <v>0.6483038417261229</v>
+        <v>0.6432697772408688</v>
       </c>
       <c r="Z58" t="n">
-        <v>0.659581587615115</v>
+        <v>0.6536885450329524</v>
       </c>
       <c r="AA58" t="n">
-        <v>0.6710306928713448</v>
+        <v>0.6642426367278365</v>
       </c>
       <c r="AB58" t="n">
-        <v>0.6826480234654282</v>
+        <v>0.674928611622971</v>
       </c>
       <c r="AC58" t="n">
-        <v>0.6944140738680578</v>
+        <v>0.6857266736909678</v>
       </c>
       <c r="AD58" t="n">
-        <v>0.7060356414440446</v>
+        <v>0.6963432186711175</v>
       </c>
       <c r="AE58" t="n">
-        <v>0.7168098455576142</v>
+        <v>0.7060744010829034</v>
       </c>
       <c r="AF58" t="n">
-        <v>0.7276454460244888</v>
+        <v>0.7158287059051542</v>
       </c>
       <c r="AG58" t="n">
-        <v>0.735726938241023</v>
+        <v>0.7227890597086009</v>
       </c>
     </row>
     <row r="59">
@@ -39433,97 +39433,97 @@
         <v>5</v>
       </c>
       <c r="C64" t="n">
-        <v>0.008717599496685359</v>
+        <v>0.015701260456910372</v>
       </c>
       <c r="D64" t="n">
-        <v>0.008708006594179508</v>
+        <v>0.014714919718700738</v>
       </c>
       <c r="E64" t="n">
-        <v>0.008701252095286948</v>
+        <v>0.013933771638654644</v>
       </c>
       <c r="F64" t="n">
-        <v>0.00869536647605533</v>
+        <v>0.013208572134835972</v>
       </c>
       <c r="G64" t="n">
-        <v>0.008689554809839135</v>
+        <v>0.012538008087178575</v>
       </c>
       <c r="H64" t="n">
-        <v>0.00868384450895068</v>
+        <v>0.011921599847089619</v>
       </c>
       <c r="I64" t="n">
-        <v>0.008678366470162428</v>
+        <v>0.011358982300288239</v>
       </c>
       <c r="J64" t="n">
-        <v>0.008674339258354523</v>
+        <v>0.010850888963237522</v>
       </c>
       <c r="K64" t="n">
-        <v>0.008670901449110521</v>
+        <v>0.010395984235291453</v>
       </c>
       <c r="L64" t="n">
-        <v>0.008667562229802655</v>
+        <v>0.00999331390870843</v>
       </c>
       <c r="M64" t="n">
-        <v>0.008664258588374657</v>
+        <v>0.009642362255549783</v>
       </c>
       <c r="N64" t="n">
-        <v>0.008661100015988398</v>
+        <v>0.00934279662938816</v>
       </c>
       <c r="O64" t="n">
-        <v>0.008659363426853755</v>
+        <v>0.009095462295731008</v>
       </c>
       <c r="P64" t="n">
-        <v>0.00865822809980632</v>
+        <v>0.008899117259318058</v>
       </c>
       <c r="Q64" t="n">
-        <v>0.008657095811096593</v>
+        <v>0.008752752293869003</v>
       </c>
       <c r="R64" t="n">
         <v>0.008655966700397134</v>
       </c>
       <c r="S64" t="n">
-        <v>0.008654839002256302</v>
+        <v>0.008608367929322663</v>
       </c>
       <c r="T64" t="n">
-        <v>0.008654946595406433</v>
+        <v>0.008610809018969658</v>
       </c>
       <c r="U64" t="n">
-        <v>0.008656068830962415</v>
+        <v>0.008662698311650067</v>
       </c>
       <c r="V64" t="n">
-        <v>0.008657186496083082</v>
+        <v>0.00876265530406626</v>
       </c>
       <c r="W64" t="n">
-        <v>0.008658301633050642</v>
+        <v>0.00891033035213811</v>
       </c>
       <c r="X64" t="n">
-        <v>0.008659414088651623</v>
+        <v>0.009105381105280913</v>
       </c>
       <c r="Y64" t="n">
-        <v>0.008661158468572771</v>
+        <v>0.009348109344982558</v>
       </c>
       <c r="Z64" t="n">
-        <v>0.008664223701535731</v>
+        <v>0.009638880432531272</v>
       </c>
       <c r="AA64" t="n">
-        <v>0.008667409953132664</v>
+        <v>0.009976180105976262</v>
       </c>
       <c r="AB64" t="n">
-        <v>0.008670610292036049</v>
+        <v>0.010359596029107528</v>
       </c>
       <c r="AC64" t="n">
-        <v>0.0086738987735279</v>
+        <v>0.010789420469940457</v>
       </c>
       <c r="AD64" t="n">
-        <v>0.008677569028853468</v>
+        <v>0.011273389146413215</v>
       </c>
       <c r="AE64" t="n">
-        <v>0.008683012875464349</v>
+        <v>0.01183522608247285</v>
       </c>
       <c r="AF64" t="n">
-        <v>0.0086887800602567</v>
+        <v>0.012452422847771129</v>
       </c>
       <c r="AG64" t="n">
-        <v>0.008695220465368995</v>
+        <v>0.013191166106525758</v>
       </c>
     </row>
     <row r="65">
@@ -39534,97 +39534,97 @@
         <v>5</v>
       </c>
       <c r="C65" t="n">
-        <v>0.033442036621157134</v>
+        <v>0.02124854737144099</v>
       </c>
       <c r="D65" t="n">
-        <v>0.033031254717572185</v>
+        <v>0.020447925403154335</v>
       </c>
       <c r="E65" t="n">
-        <v>0.032648289663847474</v>
+        <v>0.01988779123518613</v>
       </c>
       <c r="F65" t="n">
-        <v>0.03230476088401793</v>
+        <v>0.019533245125468765</v>
       </c>
       <c r="G65" t="n">
-        <v>0.03199853012126669</v>
+        <v>0.019381985137007767</v>
       </c>
       <c r="H65" t="n">
-        <v>0.031728764869972156</v>
+        <v>0.019433018600397683</v>
       </c>
       <c r="I65" t="n">
-        <v>0.03150485522868599</v>
+        <v>0.019695578940689393</v>
       </c>
       <c r="J65" t="n">
-        <v>0.03131855662056043</v>
+        <v>0.02016126837026885</v>
       </c>
       <c r="K65" t="n">
-        <v>0.03118859825117206</v>
+        <v>0.020848666318111126</v>
       </c>
       <c r="L65" t="n">
-        <v>0.031097617964674272</v>
+        <v>0.021740264257166273</v>
       </c>
       <c r="M65" t="n">
-        <v>0.031059649338098728</v>
+        <v>0.022849952766478956</v>
       </c>
       <c r="N65" t="n">
-        <v>0.031062550257763808</v>
+        <v>0.02416545007571377</v>
       </c>
       <c r="O65" t="n">
-        <v>0.031117496880891115</v>
+        <v>0.02569779599853127</v>
       </c>
       <c r="P65" t="n">
-        <v>0.031217589841424143</v>
+        <v>0.027439958102309307</v>
       </c>
       <c r="Q65" t="n">
-        <v>0.03136970876794473</v>
+        <v>0.029398686193512037</v>
       </c>
       <c r="R65" t="n">
         <v>0.03156901304912033</v>
       </c>
       <c r="S65" t="n">
-        <v>0.031820921618142414</v>
+        <v>0.03395623416653329</v>
       </c>
       <c r="T65" t="n">
-        <v>0.03212452950121403</v>
+        <v>0.03655932427705402</v>
       </c>
       <c r="U65" t="n">
-        <v>0.032485104515267246</v>
+        <v>0.03938343400819396</v>
       </c>
       <c r="V65" t="n">
-        <v>0.032904171014288754</v>
+        <v>0.04242997359422362</v>
       </c>
       <c r="W65" t="n">
-        <v>0.033380302616354524</v>
+        <v>0.04569740556711876</v>
       </c>
       <c r="X65" t="n">
-        <v>0.033918234172395444</v>
+        <v>0.04919035668896878</v>
       </c>
       <c r="Y65" t="n">
-        <v>0.03451066872308767</v>
+        <v>0.0529014248722838</v>
       </c>
       <c r="Z65" t="n">
-        <v>0.035166023859348486</v>
+        <v>0.05683892550372131</v>
       </c>
       <c r="AA65" t="n">
-        <v>0.035876962101987736</v>
+        <v>0.06099542178682077</v>
       </c>
       <c r="AB65" t="n">
-        <v>0.036653421537417734</v>
+        <v>0.06538075534068438</v>
       </c>
       <c r="AC65" t="n">
-        <v>0.03748566142381574</v>
+        <v>0.0699852543496809</v>
       </c>
       <c r="AD65" t="n">
-        <v>0.03838656511438041</v>
+        <v>0.07482415287626767</v>
       </c>
       <c r="AE65" t="n">
-        <v>0.0393466377645305</v>
+        <v>0.07989501008191598</v>
       </c>
       <c r="AF65" t="n">
-        <v>0.04037879152860064</v>
+        <v>0.08520408653864733</v>
       </c>
       <c r="AG65" t="n">
-        <v>0.04147510502833144</v>
+        <v>0.09075894636054155</v>
       </c>
     </row>
     <row r="66">
@@ -39746,97 +39746,97 @@
         <v>5</v>
       </c>
       <c r="C69" t="n">
-        <v>0.7726258123811969</v>
+        <v>0.7780438722076599</v>
       </c>
       <c r="D69" t="n">
-        <v>0.7612672917717743</v>
+        <v>0.7664872261142941</v>
       </c>
       <c r="E69" t="n">
-        <v>0.7537624444068647</v>
+        <v>0.7587932167769407</v>
       </c>
       <c r="F69" t="n">
-        <v>0.7464034916580025</v>
+        <v>0.7512239446168842</v>
       </c>
       <c r="G69" t="n">
-        <v>0.739194516336716</v>
+        <v>0.7437816427799351</v>
       </c>
       <c r="H69" t="n">
-        <v>0.7321392659556852</v>
+        <v>0.7364682363050895</v>
       </c>
       <c r="I69" t="n">
-        <v>0.7252383828837643</v>
+        <v>0.7292825721430849</v>
       </c>
       <c r="J69" t="n">
-        <v>0.7184976673744964</v>
+        <v>0.722228682045446</v>
       </c>
       <c r="K69" t="n">
-        <v>0.7119144565410986</v>
+        <v>0.715302161397557</v>
       </c>
       <c r="L69" t="n">
-        <v>0.7054965175592385</v>
+        <v>0.7085090622777095</v>
       </c>
       <c r="M69" t="n">
-        <v>0.6996649029232829</v>
+        <v>0.7022687485668274</v>
       </c>
       <c r="N69" t="n">
-        <v>0.6935568471301855</v>
+        <v>0.6957167924850057</v>
       </c>
       <c r="O69" t="n">
-        <v>0.6876182629133806</v>
+        <v>0.6892974706783005</v>
       </c>
       <c r="P69" t="n">
-        <v>0.6818533540693321</v>
+        <v>0.6830133768947296</v>
       </c>
       <c r="Q69" t="n">
-        <v>0.676262221424405</v>
+        <v>0.6768630278015326</v>
       </c>
       <c r="R69" t="n">
         <v>0.6708484406040848</v>
       </c>
       <c r="S69" t="n">
-        <v>0.6656124445209785</v>
+        <v>0.6649685153834667</v>
       </c>
       <c r="T69" t="n">
-        <v>0.660556624775646</v>
+        <v>0.6592241363469663</v>
       </c>
       <c r="U69" t="n">
-        <v>0.6556811854700082</v>
+        <v>0.6536140254914697</v>
       </c>
       <c r="V69" t="n">
-        <v>0.6509872450794878</v>
+        <v>0.6481378443260961</v>
       </c>
       <c r="W69" t="n">
-        <v>0.6464768731047108</v>
+        <v>0.6427962303750856</v>
       </c>
       <c r="X69" t="n">
-        <v>0.642150188535404</v>
+        <v>0.6375878954937573</v>
       </c>
       <c r="Y69" t="n">
-        <v>0.6380109170070098</v>
+        <v>0.6325151828782112</v>
       </c>
       <c r="Z69" t="n">
-        <v>0.634057926737887</v>
+        <v>0.6275756028568036</v>
       </c>
       <c r="AA69" t="n">
-        <v>0.6302945651638013</v>
+        <v>0.6227711693802344</v>
       </c>
       <c r="AB69" t="n">
-        <v>0.626718968135179</v>
+        <v>0.6180987090758521</v>
       </c>
       <c r="AC69" t="n">
-        <v>0.6233115599594512</v>
+        <v>0.6135373513061855</v>
       </c>
       <c r="AD69" t="n">
-        <v>0.6197549051004921</v>
+        <v>0.6087681758316077</v>
       </c>
       <c r="AE69" t="n">
-        <v>0.6152862847113735</v>
+        <v>0.6030262226511707</v>
       </c>
       <c r="AF69" t="n">
-        <v>0.6108955511071285</v>
+        <v>0.5973002814747222</v>
       </c>
       <c r="AG69" t="n">
-        <v>0.6049084388835335</v>
+        <v>0.589912864843483</v>
       </c>
     </row>
     <row r="70">
@@ -39857,97 +39857,97 @@
         <v>5</v>
       </c>
       <c r="C72" t="n">
-        <v>0.6633502664070919</v>
+        <v>0.6690234986773641</v>
       </c>
       <c r="D72" t="n">
-        <v>0.6677432929657463</v>
+        <v>0.6732002614437842</v>
       </c>
       <c r="E72" t="n">
-        <v>0.6756957470810798</v>
+        <v>0.6809402125191814</v>
       </c>
       <c r="F72" t="n">
-        <v>0.6838017748847653</v>
+        <v>0.688809393525071</v>
       </c>
       <c r="G72" t="n">
-        <v>0.6920635717035821</v>
+        <v>0.6968091959675073</v>
       </c>
       <c r="H72" t="n">
-        <v>0.7004829808962191</v>
+        <v>0.7049406858525405</v>
       </c>
       <c r="I72" t="n">
-        <v>0.7090586618964698</v>
+        <v>0.7132017714596206</v>
       </c>
       <c r="J72" t="n">
-        <v>0.7177946343715546</v>
+        <v>0.7215957472270933</v>
       </c>
       <c r="K72" t="n">
-        <v>0.7266862849819151</v>
+        <v>0.7301173002366769</v>
       </c>
       <c r="L72" t="n">
-        <v>0.7357396744647988</v>
+        <v>0.7387718170198495</v>
       </c>
       <c r="M72" t="n">
-        <v>0.7453740144911223</v>
+        <v>0.7479778601346668</v>
       </c>
       <c r="N72" t="n">
-        <v>0.7547247721625239</v>
+        <v>0.7568702723818425</v>
       </c>
       <c r="O72" t="n">
-        <v>0.7642360990972951</v>
+        <v>0.7658926056098839</v>
       </c>
       <c r="P72" t="n">
-        <v>0.7739104282035735</v>
+        <v>0.7750467172039577</v>
       </c>
       <c r="Q72" t="n">
-        <v>0.7837461570728748</v>
+        <v>0.7843304531959306</v>
       </c>
       <c r="R72" t="n">
         <v>0.7937451029549658</v>
       </c>
       <c r="S72" t="n">
-        <v>0.8039060386848823</v>
+        <v>0.8032889348300345</v>
       </c>
       <c r="T72" t="n">
-        <v>0.8142296584435045</v>
+        <v>0.812962161625992</v>
       </c>
       <c r="U72" t="n">
-        <v>0.8247145747515323</v>
+        <v>0.8227629373132642</v>
       </c>
       <c r="V72" t="n">
-        <v>0.8353602981855728</v>
+        <v>0.8326903364600593</v>
       </c>
       <c r="W72" t="n">
-        <v>0.8461672515847734</v>
+        <v>0.8427443681557246</v>
       </c>
       <c r="X72" t="n">
-        <v>0.8571340475431842</v>
+        <v>0.852923253220609</v>
       </c>
       <c r="Y72" t="n">
-        <v>0.8682626533425635</v>
+        <v>0.8632285888573095</v>
       </c>
       <c r="Z72" t="n">
-        <v>0.8795505558957115</v>
+        <v>0.8736575133135491</v>
       </c>
       <c r="AA72" t="n">
-        <v>0.8909993412031629</v>
+        <v>0.8842112850596546</v>
       </c>
       <c r="AB72" t="n">
-        <v>0.9026058752511275</v>
+        <v>0.8948864634086702</v>
       </c>
       <c r="AC72" t="n">
-        <v>0.9143506530365063</v>
+        <v>0.9056632528594163</v>
       </c>
       <c r="AD72" t="n">
-        <v>0.9259404729609076</v>
+        <v>0.9162480501879803</v>
       </c>
       <c r="AE72" t="n">
-        <v>0.9366724559358928</v>
+        <v>0.9259370114611821</v>
       </c>
       <c r="AF72" t="n">
-        <v>0.947455363834983</v>
+        <v>0.9356386237156484</v>
       </c>
       <c r="AG72" t="n">
-        <v>0.9554736946226938</v>
+        <v>0.9425358160902717</v>
       </c>
     </row>
     <row r="73">
@@ -40175,97 +40175,97 @@
         <v>5</v>
       </c>
       <c r="C78" t="n">
-        <v>0.01143759949668536</v>
+        <v>0.018421260456910372</v>
       </c>
       <c r="D78" t="n">
-        <v>0.011428006594179509</v>
+        <v>0.017434919718700738</v>
       </c>
       <c r="E78" t="n">
-        <v>0.011421252095286948</v>
+        <v>0.016653771638654644</v>
       </c>
       <c r="F78" t="n">
-        <v>0.01141536647605533</v>
+        <v>0.01592857213483597</v>
       </c>
       <c r="G78" t="n">
-        <v>0.011409554809839136</v>
+        <v>0.015258008087178573</v>
       </c>
       <c r="H78" t="n">
-        <v>0.01140384450895068</v>
+        <v>0.014641599847089619</v>
       </c>
       <c r="I78" t="n">
-        <v>0.011398366470162428</v>
+        <v>0.014078982300288239</v>
       </c>
       <c r="J78" t="n">
-        <v>0.011394339258354522</v>
+        <v>0.01357088896323752</v>
       </c>
       <c r="K78" t="n">
-        <v>0.011390901449110521</v>
+        <v>0.013115984235291454</v>
       </c>
       <c r="L78" t="n">
-        <v>0.011387562229802653</v>
+        <v>0.012713313908708428</v>
       </c>
       <c r="M78" t="n">
-        <v>0.011384258588374656</v>
+        <v>0.012362362255549783</v>
       </c>
       <c r="N78" t="n">
-        <v>0.011381100015988398</v>
+        <v>0.01206279662938816</v>
       </c>
       <c r="O78" t="n">
-        <v>0.011379363426853754</v>
+        <v>0.011815462295731008</v>
       </c>
       <c r="P78" t="n">
-        <v>0.01137822809980632</v>
+        <v>0.011619117259318058</v>
       </c>
       <c r="Q78" t="n">
-        <v>0.011377095811096593</v>
+        <v>0.011472752293869003</v>
       </c>
       <c r="R78" t="n">
         <v>0.011375966700397134</v>
       </c>
       <c r="S78" t="n">
-        <v>0.011374839002256302</v>
+        <v>0.011328367929322663</v>
       </c>
       <c r="T78" t="n">
-        <v>0.011374946595406433</v>
+        <v>0.011330809018969658</v>
       </c>
       <c r="U78" t="n">
-        <v>0.011376068830962413</v>
+        <v>0.011382698311650067</v>
       </c>
       <c r="V78" t="n">
-        <v>0.011377186496083082</v>
+        <v>0.01148265530406626</v>
       </c>
       <c r="W78" t="n">
-        <v>0.01137830163305064</v>
+        <v>0.01163033035213811</v>
       </c>
       <c r="X78" t="n">
-        <v>0.011379414088651623</v>
+        <v>0.011825381105280912</v>
       </c>
       <c r="Y78" t="n">
-        <v>0.011381158468572771</v>
+        <v>0.012068109344982557</v>
       </c>
       <c r="Z78" t="n">
-        <v>0.011384223701535731</v>
+        <v>0.012358880432531272</v>
       </c>
       <c r="AA78" t="n">
-        <v>0.011387409953132664</v>
+        <v>0.01269618010597626</v>
       </c>
       <c r="AB78" t="n">
-        <v>0.011390610292036049</v>
+        <v>0.013079596029107528</v>
       </c>
       <c r="AC78" t="n">
-        <v>0.011393898773527901</v>
+        <v>0.013509420469940457</v>
       </c>
       <c r="AD78" t="n">
-        <v>0.011397569028853468</v>
+        <v>0.013993389146413213</v>
       </c>
       <c r="AE78" t="n">
-        <v>0.011403012875464347</v>
+        <v>0.014555226082472849</v>
       </c>
       <c r="AF78" t="n">
-        <v>0.0114087800602567</v>
+        <v>0.015172422847771129</v>
       </c>
       <c r="AG78" t="n">
-        <v>0.011415220465368994</v>
+        <v>0.015911166106525758</v>
       </c>
     </row>
     <row r="79">
@@ -40276,97 +40276,97 @@
         <v>5</v>
       </c>
       <c r="C79" t="n">
-        <v>0.03430119473733941</v>
+        <v>0.022107705487623266</v>
       </c>
       <c r="D79" t="n">
-        <v>0.033890412833754456</v>
+        <v>0.021307083519336613</v>
       </c>
       <c r="E79" t="n">
-        <v>0.033507447780029745</v>
+        <v>0.020746949351368407</v>
       </c>
       <c r="F79" t="n">
-        <v>0.03316391900020021</v>
+        <v>0.020392403241651036</v>
       </c>
       <c r="G79" t="n">
-        <v>0.032857688237448966</v>
+        <v>0.02024114325319004</v>
       </c>
       <c r="H79" t="n">
-        <v>0.032587922986154434</v>
+        <v>0.02029217671657996</v>
       </c>
       <c r="I79" t="n">
-        <v>0.03236401334486827</v>
+        <v>0.020554737056871667</v>
       </c>
       <c r="J79" t="n">
-        <v>0.032177714736742705</v>
+        <v>0.021020426486451124</v>
       </c>
       <c r="K79" t="n">
-        <v>0.03204775636735433</v>
+        <v>0.021707824434293404</v>
       </c>
       <c r="L79" t="n">
-        <v>0.03195677608085654</v>
+        <v>0.02259942237334855</v>
       </c>
       <c r="M79" t="n">
-        <v>0.031918807454280995</v>
+        <v>0.02370911088266123</v>
       </c>
       <c r="N79" t="n">
-        <v>0.03192170837394609</v>
+        <v>0.02502460819189604</v>
       </c>
       <c r="O79" t="n">
-        <v>0.031976654997073396</v>
+        <v>0.02655695411471355</v>
       </c>
       <c r="P79" t="n">
-        <v>0.032076747957606414</v>
+        <v>0.028299116218491585</v>
       </c>
       <c r="Q79" t="n">
-        <v>0.03222886688412701</v>
+        <v>0.030257844309694314</v>
       </c>
       <c r="R79" t="n">
         <v>0.03242817116530261</v>
       </c>
       <c r="S79" t="n">
-        <v>0.0326800797343247</v>
+        <v>0.03481539228271557</v>
       </c>
       <c r="T79" t="n">
-        <v>0.032983687617396305</v>
+        <v>0.0374184823932363</v>
       </c>
       <c r="U79" t="n">
-        <v>0.03334426263144952</v>
+        <v>0.04024259212437624</v>
       </c>
       <c r="V79" t="n">
-        <v>0.03376332913047103</v>
+        <v>0.043289131710405895</v>
       </c>
       <c r="W79" t="n">
-        <v>0.0342394607325368</v>
+        <v>0.046556563683301036</v>
       </c>
       <c r="X79" t="n">
-        <v>0.034777392288577715</v>
+        <v>0.05004951480515105</v>
       </c>
       <c r="Y79" t="n">
-        <v>0.03536982683926994</v>
+        <v>0.053760582988466074</v>
       </c>
       <c r="Z79" t="n">
-        <v>0.036025181975530764</v>
+        <v>0.05769808361990359</v>
       </c>
       <c r="AA79" t="n">
-        <v>0.036736120218170014</v>
+        <v>0.06185457990300304</v>
       </c>
       <c r="AB79" t="n">
-        <v>0.03751257965360002</v>
+        <v>0.06623991345686667</v>
       </c>
       <c r="AC79" t="n">
-        <v>0.03834481953999802</v>
+        <v>0.07084441246586319</v>
       </c>
       <c r="AD79" t="n">
-        <v>0.03924572323056268</v>
+        <v>0.07568331099244995</v>
       </c>
       <c r="AE79" t="n">
-        <v>0.040205795880712776</v>
+        <v>0.08075416819809825</v>
       </c>
       <c r="AF79" t="n">
-        <v>0.041237949644782924</v>
+        <v>0.0860632446548296</v>
       </c>
       <c r="AG79" t="n">
-        <v>0.04233426314451371</v>
+        <v>0.09161810447672383</v>
       </c>
     </row>
     <row r="80">
@@ -40488,97 +40488,97 @@
         <v>5</v>
       </c>
       <c r="C83" t="n">
-        <v>0.8159724439779281</v>
+        <v>0.8213905038043912</v>
       </c>
       <c r="D83" t="n">
-        <v>0.8046340973552558</v>
+        <v>0.8098540316977754</v>
       </c>
       <c r="E83" t="n">
-        <v>0.7971475960897911</v>
+        <v>0.8021783684598671</v>
       </c>
       <c r="F83" t="n">
-        <v>0.7898051606589069</v>
+        <v>0.7946256136177889</v>
       </c>
       <c r="G83" t="n">
-        <v>0.7826108730691002</v>
+        <v>0.7871979995123195</v>
       </c>
       <c r="H83" t="n">
-        <v>0.7755684801171915</v>
+        <v>0.7798974504665958</v>
       </c>
       <c r="I83" t="n">
-        <v>0.7686786235453817</v>
+        <v>0.7727228128047026</v>
       </c>
       <c r="J83" t="n">
-        <v>0.7619471030697987</v>
+        <v>0.7656781177407481</v>
       </c>
       <c r="K83" t="n">
-        <v>0.7553712553555059</v>
+        <v>0.7587589602119642</v>
       </c>
       <c r="L83" t="n">
-        <v>0.7489588472193027</v>
+        <v>0.751971391937774</v>
       </c>
       <c r="M83" t="n">
-        <v>0.7431309308859917</v>
+        <v>0.7457347765295362</v>
       </c>
       <c r="N83" t="n">
-        <v>0.7370247406722747</v>
+        <v>0.7391846860270948</v>
       </c>
       <c r="O83" t="n">
-        <v>0.7310861892206614</v>
+        <v>0.7327653969855814</v>
       </c>
       <c r="P83" t="n">
-        <v>0.7253194803260187</v>
+        <v>0.7264795031514161</v>
       </c>
       <c r="Q83" t="n">
-        <v>0.719724714902443</v>
+        <v>0.7203255212795705</v>
       </c>
       <c r="R83" t="n">
         <v>0.7143054687524765</v>
       </c>
       <c r="S83" t="n">
-        <v>0.7090621750550993</v>
+        <v>0.7084182459175874</v>
       </c>
       <c r="T83" t="n">
-        <v>0.7039972257665459</v>
+        <v>0.7026647373378662</v>
       </c>
       <c r="U83" t="n">
-        <v>0.6991108254336988</v>
+        <v>0.6970436654551603</v>
       </c>
       <c r="V83" t="n">
-        <v>0.6944040930662052</v>
+        <v>0.6915546923128137</v>
       </c>
       <c r="W83" t="n">
-        <v>0.6898790987881545</v>
+        <v>0.6861984560585295</v>
       </c>
       <c r="X83" t="n">
-        <v>0.6855359623019439</v>
+        <v>0.6809736692602972</v>
       </c>
       <c r="Y83" t="n">
-        <v>0.6813784100448586</v>
+        <v>0.6758826759160599</v>
       </c>
       <c r="Z83" t="n">
-        <v>0.6774053111262344</v>
+        <v>0.670922987245151</v>
       </c>
       <c r="AA83" t="n">
-        <v>0.6736200139619049</v>
+        <v>0.6660966181783378</v>
       </c>
       <c r="AB83" t="n">
-        <v>0.6700206554714053</v>
+        <v>0.6614003964120784</v>
       </c>
       <c r="AC83" t="n">
-        <v>0.6665876611202671</v>
+        <v>0.6568134524670015</v>
       </c>
       <c r="AD83" t="n">
-        <v>0.6630035966193984</v>
+        <v>0.6520168673505141</v>
       </c>
       <c r="AE83" t="n">
-        <v>0.658505744457779</v>
+        <v>0.6462456823975761</v>
       </c>
       <c r="AF83" t="n">
-        <v>0.6540839583751564</v>
+        <v>0.64048868874275</v>
       </c>
       <c r="AG83" t="n">
-        <v>0.6480639744807617</v>
+        <v>0.6330684004407114</v>
       </c>
     </row>
     <row r="84">
@@ -40599,97 +40599,97 @@
         <v>5</v>
       </c>
       <c r="C86" t="n">
-        <v>0.7036529501170713</v>
+        <v>0.7093261823873435</v>
       </c>
       <c r="D86" t="n">
-        <v>0.7080665426510411</v>
+        <v>0.7135235111290785</v>
       </c>
       <c r="E86" t="n">
-        <v>0.7160378831930057</v>
+        <v>0.7212823486311072</v>
       </c>
       <c r="F86" t="n">
-        <v>0.7241611169541411</v>
+        <v>0.7291687355944467</v>
       </c>
       <c r="G86" t="n">
-        <v>0.732438438422632</v>
+        <v>0.7371840626865569</v>
       </c>
       <c r="H86" t="n">
-        <v>0.7408716902005175</v>
+        <v>0.7453293951568389</v>
       </c>
       <c r="I86" t="n">
-        <v>0.7494595310469232</v>
+        <v>0.7536026406100738</v>
       </c>
       <c r="J86" t="n">
-        <v>0.758205980036416</v>
+        <v>0.7620070928919546</v>
       </c>
       <c r="K86" t="n">
-        <v>0.7671064233188268</v>
+        <v>0.7705374385735886</v>
       </c>
       <c r="L86" t="n">
-        <v>0.7761669212028608</v>
+        <v>0.7791990637579116</v>
       </c>
       <c r="M86" t="n">
-        <v>0.7858066850129811</v>
+        <v>0.7884105306565256</v>
       </c>
       <c r="N86" t="n">
-        <v>0.7951611815864783</v>
+        <v>0.7973066818057968</v>
       </c>
       <c r="O86" t="n">
-        <v>0.8046745623594154</v>
+        <v>0.806331068872004</v>
       </c>
       <c r="P86" t="n">
-        <v>0.8143492601398284</v>
+        <v>0.8154855491402125</v>
       </c>
       <c r="Q86" t="n">
-        <v>0.8241836725012645</v>
+        <v>0.8247679686243201</v>
       </c>
       <c r="R86" t="n">
         <v>0.8341796167576551</v>
       </c>
       <c r="S86" t="n">
-        <v>0.8443358658903314</v>
+        <v>0.8437187620354835</v>
       </c>
       <c r="T86" t="n">
-        <v>0.8546531143085917</v>
+        <v>0.853385617491079</v>
       </c>
       <c r="U86" t="n">
-        <v>0.8651299748436656</v>
+        <v>0.8631783374053973</v>
       </c>
       <c r="V86" t="n">
-        <v>0.8757659584647874</v>
+        <v>0.873095996739274</v>
       </c>
       <c r="W86" t="n">
-        <v>0.8865614884858093</v>
+        <v>0.8831386050567606</v>
       </c>
       <c r="X86" t="n">
-        <v>0.897515178057541</v>
+        <v>0.8933043837349658</v>
       </c>
       <c r="Y86" t="n">
-        <v>0.9086289951005273</v>
+        <v>0.9035949306152732</v>
       </c>
       <c r="Z86" t="n">
-        <v>0.9199004272483514</v>
+        <v>0.9140073846661888</v>
       </c>
       <c r="AA86" t="n">
-        <v>0.9313310613042927</v>
+        <v>0.9245430051607844</v>
       </c>
       <c r="AB86" t="n">
-        <v>0.9429177641392268</v>
+        <v>0.9351983522967698</v>
       </c>
       <c r="AC86" t="n">
-        <v>0.9546410317166008</v>
+        <v>0.9459536315395108</v>
       </c>
       <c r="AD86" t="n">
-        <v>0.9662076634863996</v>
+        <v>0.9565152407134723</v>
       </c>
       <c r="AE86" t="n">
-        <v>0.9769147814903427</v>
+        <v>0.9661793370156321</v>
       </c>
       <c r="AF86" t="n">
-        <v>0.987671148813835</v>
+        <v>0.9758544086945005</v>
       </c>
       <c r="AG86" t="n">
-        <v>0.9956612647149422</v>
+        <v>0.9827233861825201</v>
       </c>
     </row>
     <row r="87">
@@ -40917,97 +40917,97 @@
         <v>5</v>
       </c>
       <c r="C92" t="n">
-        <v>0.014937599496685359</v>
+        <v>0.021921260456910372</v>
       </c>
       <c r="D92" t="n">
-        <v>0.014928006594179508</v>
+        <v>0.020934919718700738</v>
       </c>
       <c r="E92" t="n">
-        <v>0.014921252095286948</v>
+        <v>0.020153771638654644</v>
       </c>
       <c r="F92" t="n">
-        <v>0.01491536647605533</v>
+        <v>0.019428572134835974</v>
       </c>
       <c r="G92" t="n">
-        <v>0.014909554809839135</v>
+        <v>0.018758008087178576</v>
       </c>
       <c r="H92" t="n">
-        <v>0.01490384450895068</v>
+        <v>0.01814159984708962</v>
       </c>
       <c r="I92" t="n">
-        <v>0.01489836647016243</v>
+        <v>0.01757898230028824</v>
       </c>
       <c r="J92" t="n">
-        <v>0.014894339258354523</v>
+        <v>0.017070888963237524</v>
       </c>
       <c r="K92" t="n">
-        <v>0.014890901449110521</v>
+        <v>0.016615984235291453</v>
       </c>
       <c r="L92" t="n">
-        <v>0.014887562229802654</v>
+        <v>0.016213313908708428</v>
       </c>
       <c r="M92" t="n">
-        <v>0.014884258588374657</v>
+        <v>0.015862362255549784</v>
       </c>
       <c r="N92" t="n">
-        <v>0.0148811000159884</v>
+        <v>0.01556279662938816</v>
       </c>
       <c r="O92" t="n">
-        <v>0.014879363426853755</v>
+        <v>0.015315462295731008</v>
       </c>
       <c r="P92" t="n">
-        <v>0.01487822809980632</v>
+        <v>0.015119117259318058</v>
       </c>
       <c r="Q92" t="n">
-        <v>0.014877095811096593</v>
+        <v>0.014972752293869004</v>
       </c>
       <c r="R92" t="n">
         <v>0.014875966700397134</v>
       </c>
       <c r="S92" t="n">
-        <v>0.014874839002256304</v>
+        <v>0.014828367929322663</v>
       </c>
       <c r="T92" t="n">
-        <v>0.014874946595406432</v>
+        <v>0.01483080901896966</v>
       </c>
       <c r="U92" t="n">
-        <v>0.014876068830962414</v>
+        <v>0.014882698311650067</v>
       </c>
       <c r="V92" t="n">
-        <v>0.014877186496083081</v>
+        <v>0.01498265530406626</v>
       </c>
       <c r="W92" t="n">
-        <v>0.014878301633050641</v>
+        <v>0.015130330352138111</v>
       </c>
       <c r="X92" t="n">
-        <v>0.014879414088651625</v>
+        <v>0.015325381105280913</v>
       </c>
       <c r="Y92" t="n">
-        <v>0.014881158468572773</v>
+        <v>0.015568109344982558</v>
       </c>
       <c r="Z92" t="n">
-        <v>0.01488422370153573</v>
+        <v>0.015858880432531273</v>
       </c>
       <c r="AA92" t="n">
-        <v>0.014887409953132664</v>
+        <v>0.01619618010597626</v>
       </c>
       <c r="AB92" t="n">
-        <v>0.01489061029203605</v>
+        <v>0.016579596029107527</v>
       </c>
       <c r="AC92" t="n">
-        <v>0.0148938987735279</v>
+        <v>0.01700942046994046</v>
       </c>
       <c r="AD92" t="n">
-        <v>0.014897569028853468</v>
+        <v>0.017493389146413213</v>
       </c>
       <c r="AE92" t="n">
-        <v>0.014903012875464349</v>
+        <v>0.01805522608247285</v>
       </c>
       <c r="AF92" t="n">
-        <v>0.0149087800602567</v>
+        <v>0.01867242284777113</v>
       </c>
       <c r="AG92" t="n">
-        <v>0.014915220465368995</v>
+        <v>0.019411166106525757</v>
       </c>
     </row>
     <row r="93">
@@ -41018,97 +41018,97 @@
         <v>5</v>
       </c>
       <c r="C93" t="n">
-        <v>0.035406729078015134</v>
+        <v>0.02321323982829899</v>
       </c>
       <c r="D93" t="n">
-        <v>0.034995947174430185</v>
+        <v>0.022412617860012335</v>
       </c>
       <c r="E93" t="n">
-        <v>0.03461298212070547</v>
+        <v>0.02185248369204413</v>
       </c>
       <c r="F93" t="n">
-        <v>0.03426945334087593</v>
+        <v>0.02149793758232676</v>
       </c>
       <c r="G93" t="n">
-        <v>0.03396322257812469</v>
+        <v>0.021346677593865767</v>
       </c>
       <c r="H93" t="n">
-        <v>0.03369345732683016</v>
+        <v>0.021397711057255683</v>
       </c>
       <c r="I93" t="n">
-        <v>0.03346954768554399</v>
+        <v>0.021660271397547393</v>
       </c>
       <c r="J93" t="n">
-        <v>0.03328324907741843</v>
+        <v>0.022125960827126846</v>
       </c>
       <c r="K93" t="n">
-        <v>0.03315329070803006</v>
+        <v>0.022813358774969126</v>
       </c>
       <c r="L93" t="n">
-        <v>0.03306231042153227</v>
+        <v>0.02370495671402427</v>
       </c>
       <c r="M93" t="n">
-        <v>0.033024341794956724</v>
+        <v>0.024814645223336953</v>
       </c>
       <c r="N93" t="n">
-        <v>0.03302724271462181</v>
+        <v>0.02613014253257177</v>
       </c>
       <c r="O93" t="n">
-        <v>0.03308218933774912</v>
+        <v>0.02766248845538927</v>
       </c>
       <c r="P93" t="n">
-        <v>0.033182282298282136</v>
+        <v>0.029404650559167307</v>
       </c>
       <c r="Q93" t="n">
-        <v>0.03333440122480273</v>
+        <v>0.03136337865037003</v>
       </c>
       <c r="R93" t="n">
         <v>0.03353370550597833</v>
       </c>
       <c r="S93" t="n">
-        <v>0.03378561407500042</v>
+        <v>0.03592092662339129</v>
       </c>
       <c r="T93" t="n">
-        <v>0.03408922195807203</v>
+        <v>0.03852401673391202</v>
       </c>
       <c r="U93" t="n">
-        <v>0.034449796972125246</v>
+        <v>0.04134812646505196</v>
       </c>
       <c r="V93" t="n">
-        <v>0.034868863471146753</v>
+        <v>0.04439466605108162</v>
       </c>
       <c r="W93" t="n">
-        <v>0.03534499507321252</v>
+        <v>0.04766209802397676</v>
       </c>
       <c r="X93" t="n">
-        <v>0.035882926629253444</v>
+        <v>0.05115504914582678</v>
       </c>
       <c r="Y93" t="n">
-        <v>0.03647536117994567</v>
+        <v>0.05486611732914179</v>
       </c>
       <c r="Z93" t="n">
-        <v>0.037130716316206486</v>
+        <v>0.05880361796057931</v>
       </c>
       <c r="AA93" t="n">
-        <v>0.037841654558845736</v>
+        <v>0.06296011424367876</v>
       </c>
       <c r="AB93" t="n">
-        <v>0.038618113994275734</v>
+        <v>0.06734544779754238</v>
       </c>
       <c r="AC93" t="n">
-        <v>0.03945035388067374</v>
+        <v>0.0719499468065389</v>
       </c>
       <c r="AD93" t="n">
-        <v>0.04035125757123841</v>
+        <v>0.07678884533312567</v>
       </c>
       <c r="AE93" t="n">
-        <v>0.0413113302213885</v>
+        <v>0.08185970253877396</v>
       </c>
       <c r="AF93" t="n">
-        <v>0.04234348398545864</v>
+        <v>0.08716877899550533</v>
       </c>
       <c r="AG93" t="n">
-        <v>0.04343979748518944</v>
+        <v>0.09272363881739955</v>
       </c>
     </row>
     <row r="94">
@@ -41230,97 +41230,97 @@
         <v>5</v>
       </c>
       <c r="C97" t="n">
-        <v>0.8764533586036407</v>
+        <v>0.8818714184301042</v>
       </c>
       <c r="D97" t="n">
-        <v>0.8651478768315818</v>
+        <v>0.8703678111741013</v>
       </c>
       <c r="E97" t="n">
-        <v>0.8576915926191517</v>
+        <v>0.8627223649892279</v>
       </c>
       <c r="F97" t="n">
-        <v>0.8503767249709864</v>
+        <v>0.8551971779298686</v>
       </c>
       <c r="G97" t="n">
-        <v>0.8432073545499679</v>
+        <v>0.8477944809931872</v>
       </c>
       <c r="H97" t="n">
-        <v>0.8361872269384895</v>
+        <v>0.8405161972878942</v>
       </c>
       <c r="I97" t="n">
-        <v>0.8293169827935711</v>
+        <v>0.8333611720528917</v>
       </c>
       <c r="J97" t="n">
-        <v>0.8226024208754578</v>
+        <v>0.8263334355464071</v>
       </c>
       <c r="K97" t="n">
-        <v>0.816040877022677</v>
+        <v>0.8194285818791358</v>
       </c>
       <c r="L97" t="n">
-        <v>0.8096401173548791</v>
+        <v>0.8126526620733501</v>
       </c>
       <c r="M97" t="n">
-        <v>0.8038211935291351</v>
+        <v>0.8064250391726797</v>
       </c>
       <c r="N97" t="n">
-        <v>0.7977213394238658</v>
+        <v>0.7998812847786859</v>
       </c>
       <c r="O97" t="n">
-        <v>0.791786467372768</v>
+        <v>0.7934656751376881</v>
       </c>
       <c r="P97" t="n">
-        <v>0.786020780991379</v>
+        <v>0.7871808038167764</v>
       </c>
       <c r="Q97" t="n">
-        <v>0.78042438114396</v>
+        <v>0.7810251875210874</v>
       </c>
       <c r="R97" t="n">
         <v>0.7750008437127125</v>
       </c>
       <c r="S97" t="n">
-        <v>0.7697506020857676</v>
+        <v>0.7691066729482556</v>
       </c>
       <c r="T97" t="n">
-        <v>0.7646760485579923</v>
+        <v>0.7633435601293124</v>
       </c>
       <c r="U97" t="n">
-        <v>0.7597773881443657</v>
+        <v>0.7577102281658273</v>
       </c>
       <c r="V97" t="n">
-        <v>0.7550557404520744</v>
+        <v>0.7522063396986827</v>
       </c>
       <c r="W97" t="n">
-        <v>0.7505131763321593</v>
+        <v>0.7468325336025343</v>
       </c>
       <c r="X97" t="n">
-        <v>0.7461498163433478</v>
+        <v>0.7415875233017009</v>
       </c>
       <c r="Y97" t="n">
-        <v>0.7419693879085891</v>
+        <v>0.7364736537797905</v>
       </c>
       <c r="Z97" t="n">
-        <v>0.7379707612521722</v>
+        <v>0.7314884373710886</v>
       </c>
       <c r="AA97" t="n">
-        <v>0.734157286034116</v>
+        <v>0.7266338902505491</v>
       </c>
       <c r="AB97" t="n">
-        <v>0.7305271005473152</v>
+        <v>0.7219068414879884</v>
       </c>
       <c r="AC97" t="n">
-        <v>0.727060631759765</v>
+        <v>0.717286423106499</v>
       </c>
       <c r="AD97" t="n">
-        <v>0.7234404470138708</v>
+        <v>0.7124537177449861</v>
       </c>
       <c r="AE97" t="n">
-        <v>0.7189038305590613</v>
+        <v>0.7066437684988583</v>
       </c>
       <c r="AF97" t="n">
-        <v>0.7144406380244014</v>
+        <v>0.7008453683919952</v>
       </c>
       <c r="AG97" t="n">
-        <v>0.7083766075372144</v>
+        <v>0.6933810334971642</v>
       </c>
     </row>
     <row r="98">
@@ -41341,97 +41341,97 @@
         <v>5</v>
       </c>
       <c r="C100" t="n">
-        <v>0.7597208075750855</v>
+        <v>0.7653940398453579</v>
       </c>
       <c r="D100" t="n">
-        <v>0.7641675392094194</v>
+        <v>0.769624507687457</v>
       </c>
       <c r="E100" t="n">
-        <v>0.7721695861269837</v>
+        <v>0.7774140515650853</v>
       </c>
       <c r="F100" t="n">
-        <v>0.7803210920423682</v>
+        <v>0.7853287106826741</v>
       </c>
       <c r="G100" t="n">
-        <v>0.7886242500658122</v>
+        <v>0.7933698743297373</v>
       </c>
       <c r="H100" t="n">
-        <v>0.7970809015401186</v>
+        <v>0.8015386064964405</v>
       </c>
       <c r="I100" t="n">
-        <v>0.8056897040839444</v>
+        <v>0.8098328136470954</v>
       </c>
       <c r="J100" t="n">
-        <v>0.814454675750213</v>
+        <v>0.8182557886057517</v>
       </c>
       <c r="K100" t="n">
-        <v>0.8233712017859857</v>
+        <v>0.8268022170407476</v>
       </c>
       <c r="L100" t="n">
-        <v>0.832445341716118</v>
+        <v>0.8354774842711685</v>
       </c>
       <c r="M100" t="n">
-        <v>0.8420963062001772</v>
+        <v>0.8447001518437217</v>
       </c>
       <c r="N100" t="n">
-        <v>0.8514595615295505</v>
+        <v>0.853605061748869</v>
       </c>
       <c r="O100" t="n">
-        <v>0.8609792587134107</v>
+        <v>0.8626357652259994</v>
       </c>
       <c r="P100" t="n">
-        <v>0.8706578302519413</v>
+        <v>0.8717941192523252</v>
       </c>
       <c r="Q100" t="n">
-        <v>0.8804936735298876</v>
+        <v>0.8810779696529434</v>
       </c>
       <c r="R100" t="n">
         <v>0.8904886057914403</v>
       </c>
       <c r="S100" t="n">
-        <v>0.9006414000672539</v>
+        <v>0.9000242962124061</v>
       </c>
       <c r="T100" t="n">
-        <v>0.9109527509350115</v>
+        <v>0.9096852541174988</v>
       </c>
       <c r="U100" t="n">
-        <v>0.9214212715133812</v>
+        <v>0.9194696340751128</v>
       </c>
       <c r="V100" t="n">
-        <v>0.9320464731780741</v>
+        <v>0.9293765114525605</v>
       </c>
       <c r="W100" t="n">
-        <v>0.9428287797684405</v>
+        <v>0.939405896339392</v>
       </c>
       <c r="X100" t="n">
-        <v>0.953766805079782</v>
+        <v>0.9495560107572066</v>
       </c>
       <c r="Y100" t="n">
-        <v>0.9648625177960963</v>
+        <v>0.9598284533108422</v>
       </c>
       <c r="Z100" t="n">
-        <v>0.9761134064333464</v>
+        <v>0.9702203638511837</v>
       </c>
       <c r="AA100" t="n">
-        <v>0.987521058796073</v>
+        <v>0.9807330026525647</v>
       </c>
       <c r="AB100" t="n">
-        <v>0.999082342875248</v>
+        <v>0.9913629310327909</v>
       </c>
       <c r="AC100" t="n">
-        <v>1.0107777558731919</v>
+        <v>1.0020903556961018</v>
       </c>
       <c r="AD100" t="n">
-        <v>1.0223140985974828</v>
+        <v>1.0126216758245554</v>
       </c>
       <c r="AE100" t="n">
-        <v>1.0329884945660857</v>
+        <v>1.022253050091375</v>
       </c>
       <c r="AF100" t="n">
-        <v>1.0437097084592308</v>
+        <v>1.0318929683398963</v>
       </c>
       <c r="AG100" t="n">
-        <v>1.0516622412483128</v>
+        <v>1.0387243627158906</v>
       </c>
     </row>
     <row r="101">
@@ -41659,97 +41659,97 @@
         <v>5</v>
       </c>
       <c r="C106" t="n">
-        <v>0.01921759949668536</v>
+        <v>0.026201260456910375</v>
       </c>
       <c r="D106" t="n">
-        <v>0.01920800659417951</v>
+        <v>0.02521491971870074</v>
       </c>
       <c r="E106" t="n">
-        <v>0.01920125209528695</v>
+        <v>0.024433771638654643</v>
       </c>
       <c r="F106" t="n">
-        <v>0.019195366476055332</v>
+        <v>0.023708572134835973</v>
       </c>
       <c r="G106" t="n">
-        <v>0.019189554809839138</v>
+        <v>0.023038008087178576</v>
       </c>
       <c r="H106" t="n">
-        <v>0.01918384450895068</v>
+        <v>0.02242159984708962</v>
       </c>
       <c r="I106" t="n">
-        <v>0.01917836647016243</v>
+        <v>0.021858982300288238</v>
       </c>
       <c r="J106" t="n">
-        <v>0.019174339258354524</v>
+        <v>0.021350888963237523</v>
       </c>
       <c r="K106" t="n">
-        <v>0.019170901449110524</v>
+        <v>0.020895984235291452</v>
       </c>
       <c r="L106" t="n">
-        <v>0.019167562229802655</v>
+        <v>0.02049331390870843</v>
       </c>
       <c r="M106" t="n">
-        <v>0.019164258588374658</v>
+        <v>0.020142362255549783</v>
       </c>
       <c r="N106" t="n">
-        <v>0.0191611000159884</v>
+        <v>0.019842796629388162</v>
       </c>
       <c r="O106" t="n">
-        <v>0.019159363426853756</v>
+        <v>0.01959546229573101</v>
       </c>
       <c r="P106" t="n">
-        <v>0.019158228099806322</v>
+        <v>0.01939911725931806</v>
       </c>
       <c r="Q106" t="n">
-        <v>0.019157095811096595</v>
+        <v>0.019252752293869003</v>
       </c>
       <c r="R106" t="n">
         <v>0.019155966700397133</v>
       </c>
       <c r="S106" t="n">
-        <v>0.019154839002256303</v>
+        <v>0.019108367929322665</v>
       </c>
       <c r="T106" t="n">
-        <v>0.019154946595406435</v>
+        <v>0.01911080901896966</v>
       </c>
       <c r="U106" t="n">
-        <v>0.019156068830962415</v>
+        <v>0.019162698311650066</v>
       </c>
       <c r="V106" t="n">
-        <v>0.019157186496083084</v>
+        <v>0.019262655304066262</v>
       </c>
       <c r="W106" t="n">
-        <v>0.019158301633050642</v>
+        <v>0.01941033035213811</v>
       </c>
       <c r="X106" t="n">
-        <v>0.019159414088651624</v>
+        <v>0.019605381105280914</v>
       </c>
       <c r="Y106" t="n">
-        <v>0.019161158468572772</v>
+        <v>0.01984810934498256</v>
       </c>
       <c r="Z106" t="n">
-        <v>0.019164223701535733</v>
+        <v>0.020138880432531273</v>
       </c>
       <c r="AA106" t="n">
-        <v>0.019167409953132666</v>
+        <v>0.020476180105976263</v>
       </c>
       <c r="AB106" t="n">
-        <v>0.01917061029203605</v>
+        <v>0.02085959602910753</v>
       </c>
       <c r="AC106" t="n">
-        <v>0.019173898773527903</v>
+        <v>0.021289420469940458</v>
       </c>
       <c r="AD106" t="n">
-        <v>0.019177569028853467</v>
+        <v>0.021773389146413216</v>
       </c>
       <c r="AE106" t="n">
-        <v>0.01918301287546435</v>
+        <v>0.02233522608247285</v>
       </c>
       <c r="AF106" t="n">
-        <v>0.0191887800602567</v>
+        <v>0.02295242284777113</v>
       </c>
       <c r="AG106" t="n">
-        <v>0.019195220465368996</v>
+        <v>0.02369116610652576</v>
       </c>
     </row>
     <row r="107">
@@ -41760,97 +41760,97 @@
         <v>5</v>
       </c>
       <c r="C107" t="n">
-        <v>0.0367586396431843</v>
+        <v>0.02456515039346816</v>
       </c>
       <c r="D107" t="n">
-        <v>0.03634785773959935</v>
+        <v>0.023764528425181505</v>
       </c>
       <c r="E107" t="n">
-        <v>0.03596489268587464</v>
+        <v>0.023204394257213296</v>
       </c>
       <c r="F107" t="n">
-        <v>0.035621363906045096</v>
+        <v>0.02284984814749593</v>
       </c>
       <c r="G107" t="n">
-        <v>0.035315133143293855</v>
+        <v>0.022698588159034937</v>
       </c>
       <c r="H107" t="n">
-        <v>0.03504536789199932</v>
+        <v>0.02274962162242485</v>
       </c>
       <c r="I107" t="n">
-        <v>0.03482145825071316</v>
+        <v>0.02301218196271656</v>
       </c>
       <c r="J107" t="n">
-        <v>0.03463515964258759</v>
+        <v>0.023477871392296016</v>
       </c>
       <c r="K107" t="n">
-        <v>0.03450520127319922</v>
+        <v>0.024165269340138292</v>
       </c>
       <c r="L107" t="n">
-        <v>0.034414220986701445</v>
+        <v>0.025056867279193443</v>
       </c>
       <c r="M107" t="n">
-        <v>0.03437625236012589</v>
+        <v>0.026166555788506126</v>
       </c>
       <c r="N107" t="n">
-        <v>0.034379153279790985</v>
+        <v>0.027482053097740936</v>
       </c>
       <c r="O107" t="n">
-        <v>0.034434099902918285</v>
+        <v>0.029014399020558444</v>
       </c>
       <c r="P107" t="n">
-        <v>0.0345341928634513</v>
+        <v>0.03075656112433648</v>
       </c>
       <c r="Q107" t="n">
-        <v>0.034686311789971905</v>
+        <v>0.0327152892155392</v>
       </c>
       <c r="R107" t="n">
         <v>0.0348856160711475</v>
       </c>
       <c r="S107" t="n">
-        <v>0.03513752464016959</v>
+        <v>0.03727283718856046</v>
       </c>
       <c r="T107" t="n">
-        <v>0.035441132523241194</v>
+        <v>0.039875927299081196</v>
       </c>
       <c r="U107" t="n">
-        <v>0.03580170753729441</v>
+        <v>0.042700037030221134</v>
       </c>
       <c r="V107" t="n">
-        <v>0.03622077403631593</v>
+        <v>0.045746576616250784</v>
       </c>
       <c r="W107" t="n">
-        <v>0.0366969056383817</v>
+        <v>0.049014008589145924</v>
       </c>
       <c r="X107" t="n">
-        <v>0.0372348371944226</v>
+        <v>0.052506959710995955</v>
       </c>
       <c r="Y107" t="n">
-        <v>0.03782727174511484</v>
+        <v>0.05621802789431096</v>
       </c>
       <c r="Z107" t="n">
-        <v>0.03848262688137566</v>
+        <v>0.06015552852574848</v>
       </c>
       <c r="AA107" t="n">
-        <v>0.03919356512401491</v>
+        <v>0.06431202480884793</v>
       </c>
       <c r="AB107" t="n">
-        <v>0.03997002455944491</v>
+        <v>0.06869735836271156</v>
       </c>
       <c r="AC107" t="n">
-        <v>0.040802264445842916</v>
+        <v>0.07330185737170808</v>
       </c>
       <c r="AD107" t="n">
-        <v>0.04170316813640757</v>
+        <v>0.07814075589829483</v>
       </c>
       <c r="AE107" t="n">
-        <v>0.04266324078655767</v>
+        <v>0.08321161310394314</v>
       </c>
       <c r="AF107" t="n">
-        <v>0.04369539455062781</v>
+        <v>0.08852068956067449</v>
       </c>
       <c r="AG107" t="n">
-        <v>0.0447917080503586</v>
+        <v>0.09407554938256872</v>
       </c>
     </row>
     <row r="108">
@@ -41972,97 +41972,97 @@
         <v>5</v>
       </c>
       <c r="C111" t="n">
-        <v>0.9709648127875483</v>
+        <v>0.9763828726140114</v>
       </c>
       <c r="D111" t="n">
-        <v>0.9597242504391867</v>
+        <v>0.9649441847817066</v>
       </c>
       <c r="E111" t="n">
-        <v>0.9523285886886306</v>
+        <v>0.9573593610587068</v>
       </c>
       <c r="F111" t="n">
-        <v>0.9450700435858621</v>
+        <v>0.9498904965447441</v>
       </c>
       <c r="G111" t="n">
-        <v>0.9379526930486823</v>
+        <v>0.9425398194919019</v>
       </c>
       <c r="H111" t="n">
-        <v>0.9309802801241093</v>
+        <v>0.9353092504735142</v>
       </c>
       <c r="I111" t="n">
-        <v>0.924153443143616</v>
+        <v>0.9281976324029364</v>
       </c>
       <c r="J111" t="n">
-        <v>0.9174779787518431</v>
+        <v>0.9212089934227925</v>
       </c>
       <c r="K111" t="n">
-        <v>0.9109512208817605</v>
+        <v>0.9143389257382191</v>
       </c>
       <c r="L111" t="n">
-        <v>0.9045809339575981</v>
+        <v>0.9075934786760693</v>
       </c>
       <c r="M111" t="n">
-        <v>0.8987881681512289</v>
+        <v>0.9013920137947733</v>
       </c>
       <c r="N111" t="n">
-        <v>0.892710156066169</v>
+        <v>0.8948701014209891</v>
       </c>
       <c r="O111" t="n">
-        <v>0.8867928089715652</v>
+        <v>0.888472016736485</v>
       </c>
       <c r="P111" t="n">
-        <v>0.8810403296288135</v>
+        <v>0.8822003524542109</v>
       </c>
       <c r="Q111" t="n">
-        <v>0.8754528182584829</v>
+        <v>0.8760536246356103</v>
       </c>
       <c r="R111" t="n">
         <v>0.8700338503095629</v>
       </c>
       <c r="S111" t="n">
-        <v>0.8647838589474739</v>
+        <v>0.8641399298099619</v>
       </c>
       <c r="T111" t="n">
-        <v>0.8597052364548861</v>
+        <v>0.8583727480262061</v>
       </c>
       <c r="U111" t="n">
-        <v>0.8547981880450941</v>
+        <v>0.8527310280665555</v>
       </c>
       <c r="V111" t="n">
-        <v>0.8500638337341033</v>
+        <v>0.8472144329807116</v>
       </c>
       <c r="W111" t="n">
-        <v>0.8455042449922576</v>
+        <v>0.8418236022626326</v>
       </c>
       <c r="X111" t="n">
-        <v>0.84111954320804</v>
+        <v>0.8365572501663935</v>
       </c>
       <c r="Y111" t="n">
-        <v>0.8369134568445695</v>
+        <v>0.831417722715771</v>
       </c>
       <c r="Z111" t="n">
-        <v>0.8328848573766654</v>
+        <v>0.826402533495582</v>
       </c>
       <c r="AA111" t="n">
-        <v>0.8290370959251802</v>
+        <v>0.8215137001416131</v>
       </c>
       <c r="AB111" t="n">
-        <v>0.8253683124540697</v>
+        <v>0.8167480533947432</v>
       </c>
       <c r="AC111" t="n">
-        <v>0.8218589358125421</v>
+        <v>0.8120847271592762</v>
       </c>
       <c r="AD111" t="n">
-        <v>0.8181915354342698</v>
+        <v>0.8072048061653854</v>
       </c>
       <c r="AE111" t="n">
-        <v>0.8136033978699057</v>
+        <v>0.8013433358097027</v>
       </c>
       <c r="AF111" t="n">
-        <v>0.8090843812595804</v>
+        <v>0.7954891116271742</v>
       </c>
       <c r="AG111" t="n">
-        <v>0.802960226451404</v>
+        <v>0.7879646524113539</v>
       </c>
     </row>
     <row r="112">
@@ -42083,97 +42083,97 @@
         <v>5</v>
       </c>
       <c r="C114" t="n">
-        <v>0.8470587017494994</v>
+        <v>0.8527319340197718</v>
       </c>
       <c r="D114" t="n">
-        <v>0.8515698639790297</v>
+        <v>0.8570268324570673</v>
       </c>
       <c r="E114" t="n">
-        <v>0.8596323941829851</v>
+        <v>0.8648768596210864</v>
       </c>
       <c r="F114" t="n">
-        <v>0.8678404331280869</v>
+        <v>0.8728480517683925</v>
       </c>
       <c r="G114" t="n">
-        <v>0.8761961711692338</v>
+        <v>0.8809417954331591</v>
       </c>
       <c r="H114" t="n">
-        <v>0.8847014470865533</v>
+        <v>0.8891591520428748</v>
       </c>
       <c r="I114" t="n">
-        <v>0.8933549161288148</v>
+        <v>0.8974980256919658</v>
       </c>
       <c r="J114" t="n">
-        <v>0.90216059417196</v>
+        <v>0.9059617070274989</v>
       </c>
       <c r="K114" t="n">
-        <v>0.9111138644790796</v>
+        <v>0.9145448797338414</v>
       </c>
       <c r="L114" t="n">
-        <v>0.9202207847841639</v>
+        <v>0.9232529273392147</v>
       </c>
       <c r="M114" t="n">
-        <v>0.929900564149112</v>
+        <v>0.9325044097926564</v>
       </c>
       <c r="N114" t="n">
-        <v>0.9392886674609138</v>
+        <v>0.9414341676802322</v>
       </c>
       <c r="O114" t="n">
-        <v>0.9488292445176862</v>
+        <v>0.9504857510302751</v>
       </c>
       <c r="P114" t="n">
-        <v>0.9585247268019581</v>
+        <v>0.959661015802342</v>
       </c>
       <c r="Q114" t="n">
-        <v>0.9683735108742683</v>
+        <v>0.968957806997324</v>
       </c>
       <c r="R114" t="n">
         <v>0.9783774133480918</v>
       </c>
       <c r="S114" t="n">
-        <v>0.9885352068168869</v>
+        <v>0.987918102962039</v>
       </c>
       <c r="T114" t="n">
-        <v>0.9988475856146837</v>
+        <v>0.9975800887971711</v>
       </c>
       <c r="U114" t="n">
-        <v>1.0093131628100502</v>
+        <v>1.007361525371782</v>
       </c>
       <c r="V114" t="n">
-        <v>1.0199314499221543</v>
+        <v>1.017261488196641</v>
       </c>
       <c r="W114" t="n">
-        <v>1.0307028711273516</v>
+        <v>1.0272799876983032</v>
       </c>
       <c r="X114" t="n">
-        <v>1.0416260407514815</v>
+        <v>1.0374152464289061</v>
       </c>
       <c r="Y114" t="n">
-        <v>1.0527029282025873</v>
+        <v>1.0476688637173335</v>
       </c>
       <c r="Z114" t="n">
-        <v>1.0639310229141494</v>
+        <v>1.0580379803319866</v>
       </c>
       <c r="AA114" t="n">
-        <v>1.0753119138016516</v>
+        <v>1.068523857658143</v>
       </c>
       <c r="AB114" t="n">
-        <v>1.0868424701603818</v>
+        <v>1.0791230583179252</v>
       </c>
       <c r="AC114" t="n">
-        <v>1.0985031906902878</v>
+        <v>1.089815790513198</v>
       </c>
       <c r="AD114" t="n">
-        <v>1.1100008778898085</v>
+        <v>1.1003084551168811</v>
       </c>
       <c r="AE114" t="n">
-        <v>1.120632657160925</v>
+        <v>1.1098972126862143</v>
       </c>
       <c r="AF114" t="n">
-        <v>1.1313072952609453</v>
+        <v>1.1194905551416108</v>
       </c>
       <c r="AG114" t="n">
-        <v>1.1392092954313027</v>
+        <v>1.1262714168988803</v>
       </c>
     </row>
   </sheetData>
@@ -42420,7 +42420,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.23286873770200842</v>
+        <v>-0.22937249042563274</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -42461,7 +42461,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.12117721163163592</v>
+        <v>-0.1200728626523424</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -42502,7 +42502,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0052775994966853595</v>
+        <v>0.012261260456910372</v>
       </c>
       <c r="D7"/>
       <c r="E7"/>
@@ -42543,7 +42543,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>0.032355454297750136</v>
+        <v>0.020161965048033994</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
@@ -42584,7 +42584,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>1.491783045657948</v>
+        <v>1.5622558863143565</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
@@ -42625,7 +42625,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>0.36410493106125896</v>
+        <v>0.36832045657980395</v>
       </c>
       <c r="D10"/>
       <c r="E10"/>
@@ -42666,7 +42666,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.264104931061259</v>
+        <v>-0.2683204565798039</v>
       </c>
       <c r="D11"/>
       <c r="E11"/>
@@ -42707,7 +42707,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>-3.745186530731608</v>
+        <v>-5.955414681370593</v>
       </c>
       <c r="D12"/>
       <c r="E12"/>
@@ -42748,7 +42748,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>31.679241643033222</v>
+        <v>19.012892248115016</v>
       </c>
     </row>
     <row r="14">
@@ -42769,7 +42769,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.26735547292781336</v>
+        <v>-0.2632682306469078</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -42810,7 +42810,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.1320704316573269</v>
+        <v>-0.1307794068858404</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -42851,7 +42851,7 @@
         <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0052775994966853595</v>
+        <v>0.012261260456910372</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -42892,7 +42892,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>0.032355454297750136</v>
+        <v>0.020161965048033994</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -42933,7 +42933,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7966439424400225</v>
+        <v>0.879029297713001</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
@@ -42974,7 +42974,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>0.32980260775750186</v>
+        <v>0.3340930915505447</v>
       </c>
       <c r="D21"/>
       <c r="E21"/>
@@ -43015,7 +43015,7 @@
         <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>0.07019739224249814</v>
+        <v>0.06590690844945533</v>
       </c>
       <c r="D22"/>
       <c r="E22"/>
@@ -43056,7 +43056,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>-4.081859906584916</v>
+        <v>-6.486441503805343</v>
       </c>
       <c r="D23"/>
       <c r="E23"/>
@@ -43097,7 +43097,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>34.65218623424504</v>
+        <v>20.73087579819923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>